<commit_message>
Angular - 01.INTRO TO ANGULAR AND TYPESCRIPT - Complete
</commit_message>
<xml_diff>
--- a/Angular/Angular - ноември 2020/Angular.xlsx
+++ b/Angular/Angular - ноември 2020/Angular.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
   <si>
     <t>tsc myfile.ts</t>
   </si>
@@ -144,6 +144,15 @@
   </si>
   <si>
     <t>Дефиниции за TypeScript</t>
+  </si>
+  <si>
+    <t>.\node_modules\.bin\tsc index.ts</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> .\node_modules\.bin\tsc -t es5 6.KeyValuePairs.ts</t>
+  </si>
+  <si>
+    <t>To compile your code with for target version of es 5</t>
   </si>
 </sst>
 </file>
@@ -216,11 +225,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -494,7 +503,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -502,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -513,16 +522,17 @@
     <col min="1" max="1" width="21.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="35" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="52.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -530,7 +540,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>24</v>
       </c>
@@ -538,18 +548,18 @@
         <v>25</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>18</v>
       </c>
@@ -560,7 +570,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
@@ -570,79 +580,94 @@
       <c r="C6" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1"/>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+    <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+    <row r="14" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-    </row>
-    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A8:C8"/>
-    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="A14:C14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Angular - Update xlsx
</commit_message>
<xml_diff>
--- a/Angular/Angular - ноември 2020/Angular.xlsx
+++ b/Angular/Angular - ноември 2020/Angular.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="1.Angular-Introduction" sheetId="1" r:id="rId1"/>
+    <sheet name="02.Components" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="154">
   <si>
     <t>tsc myfile.ts</t>
   </si>
@@ -153,6 +154,721 @@
   </si>
   <si>
     <t>To compile your code with for target version of es 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Creating Components Manually </t>
+  </si>
+  <si>
+    <t xml:space="preserve">import { Component } from '@angular/core';
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">To create a component we need the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Component</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> decorator</t>
+    </r>
+  </si>
+  <si>
+    <t>It provides metadata and tells Angular that we are    creating a Component and not an ordinary class</t>
+  </si>
+  <si>
+    <t>"@Component({
+   selector: 'app-home',
+   template: '&lt;h1&gt;Home View&lt;/h1&gt;'
+})"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We call it whilist adding '@' 
+in front and pass in metadata
+</t>
+  </si>
+  <si>
+    <t>Component Metadata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">selector: 'app-home'
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">selector </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- the component's HTML selector</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>template or templateUrl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - the component's template</t>
+    </r>
+  </si>
+  <si>
+    <t>templateUrl: 'Path to template'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>styles or styleUrls</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - unique styles for the current                                        component</t>
+    </r>
+  </si>
+  <si>
+    <t>styleUrls: 'Array of paths'</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>providers</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - list of providers that can be injected using DI</t>
+    </r>
+  </si>
+  <si>
+    <t>After the creation of a component we need to add it in the declarations array at the app module</t>
+  </si>
+  <si>
+    <t>NgModules help organize an application into                             cohesive blocks of functionality</t>
+  </si>
+  <si>
+    <t>"@NgModule({
+ declarations: [
+  AppComponent,
+  HomeComponent
+ ]
+})"</t>
+  </si>
+  <si>
+    <t>Creating Components with the CLI</t>
+  </si>
+  <si>
+    <t>We can use the Angular CLI to generate a new component</t>
+  </si>
+  <si>
+    <t>The CLI creates a new folder src/app/home/</t>
+  </si>
+  <si>
+    <t>The CLI directly imports the component in the app module</t>
+  </si>
+  <si>
+    <t>Bootstrapping - Starting the Application</t>
+  </si>
+  <si>
+    <t>Bootstrapping an Application</t>
+  </si>
+  <si>
+    <t>An NgModule class describes how the application parts fit together</t>
+  </si>
+  <si>
+    <t>platformBrowserDynamic().bootstrapModule(AppModule)</t>
+  </si>
+  <si>
+    <t>Every application has at least one NgModule – the root module. It is used to bootstrap (launch) the application</t>
+  </si>
+  <si>
+    <t>Usually it is called AppModule, but it is not necessary</t>
+  </si>
+  <si>
+    <t>The Initial Module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">import { BrowserModule } from '@angular/platform-browser';
+import { NgModule } from '@angular/core';
+import { AppComponent } from './app.component';
+</t>
+  </si>
+  <si>
+    <t>"@NgModule({
+declarations: [ AppComponent ],
+imports: [ BrowserModule ],
+providers: [],
+bootstrap: [ AppComponent ]
+})"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The @NgModule tells Angular how to compile and launch the app
+</t>
+  </si>
+  <si>
+    <t>export class AppModule { }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The declarations array </t>
+  </si>
+  <si>
+    <t>Only declarables – (components, directives and pipes)</t>
+  </si>
+  <si>
+    <t>The imports array</t>
+  </si>
+  <si>
+    <t>Only @NgModule classes – integrated (HttpClientModule,  BrowserModule) or custom made</t>
+  </si>
+  <si>
+    <t>The providers array</t>
+  </si>
+  <si>
+    <t>Register service providers and inject them into components</t>
+  </si>
+  <si>
+    <t>The bootstrap array</t>
+  </si>
+  <si>
+    <t>The root component – used to launch the application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Inserting a bootstrapped component                                               usually triggers a cascade of component creation </t>
+  </si>
+  <si>
+    <t>Data Bindings &amp; Templates</t>
+  </si>
+  <si>
+    <t>render nested properties of an object</t>
+  </si>
+  <si>
+    <t>attach events and handle them in the component</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">render array properties using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*ngFor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> repeater</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">condition statements using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>*ngIf</t>
+    </r>
+  </si>
+  <si>
+    <t>A template is a form of HTML that tells Angular how to render the component. Templates can be both inline or in a separate file</t>
+  </si>
+  <si>
+    <t>Render an Array Using *NgFor</t>
+  </si>
+  <si>
+    <t>export class GamesComponent {
+  games : Game[];   constructor() { 
+    this.games = [ // Array of games ]
+  }
+}</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;Games List&lt;/h1&gt;
+  &lt;p&gt;Pick a game to Buy&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li *ngFor="let game of games"&gt;
+    {{game.title}}
+  &lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The '*' symbol is  required in front
+</t>
+  </si>
+  <si>
+    <t>Conditional Statements Using *NgIf</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;Games List&lt;/h1&gt;
+&lt;p&gt;Pick a game to Buy&lt;/p&gt;
+&lt;ul&gt;
+  &lt;li *ngFor="let game of games"&gt;
+   &lt;div&gt;
+    {{game.title}}
+   &lt;/div&gt;
+   &lt;span *ngIf="game.price &gt;= 100"&gt;
+ Price: {{game.price}}
+   &lt;/span&gt;
+  &lt;/li&gt;
+&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>Attach Events</t>
+  </si>
+  <si>
+    <t>export class GamesComponent {
+    public games: Game[];
+    showContent: boolean;
+     constructor() {
+      this.games = [ // Array of games ]
+    }
+     showAdditionalContent($event) {
+   this.showContent = true;
+    }
+}</t>
+  </si>
+  <si>
+    <t>Binding Attributes</t>
+  </si>
+  <si>
+    <t>export class GamesComponent {
+   imgUrl: string;    constructor() {
+    this.imgUrl = "a url to an image"
+   }
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The name of the property in the component
+</t>
+  </si>
+  <si>
+    <t>Binding CSS Classes or Specific Class Name</t>
+  </si>
+  <si>
+    <t>You can bind to a specific class name</t>
+  </si>
+  <si>
+    <t>Binding classes</t>
+  </si>
+  <si>
+    <t>&lt;div [class]="badCurly"&gt;Bad curly&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>&lt;div [class.special]="isSpecial"&gt;
+ The class binding is special
+&lt;/div&gt;
+&lt;div class="special"[class.special]="!isSpecial"&gt;
+ This one is not so special
+&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Binding styles</t>
+  </si>
+  <si>
+    <t>&lt;button [style.color]="isSpecial ? 'red': 'green'"&gt;Red&lt;/button&gt;
+&lt;button [style.background-color]="canSave ? 'cyan': 'grey'" &gt;
+ Save
+&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>Or styles with units</t>
+  </si>
+  <si>
+    <t>&lt;button [style.font-size.em]="isSpecial ? 3 : 1"&gt;
+ Big
+&lt;/button&gt;
+&lt;button [style.font-size.%]="!isSpecial ? 150 : 50"&gt;
+ Small
+&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>Reference other elements</t>
+  </si>
+  <si>
+    <t>&lt;input #phone placeholder="phone number"&gt;
+&lt;button (click)="callPhone(phone.value)"&gt;Call&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t>phone refers to the input element</t>
+  </si>
+  <si>
+    <t>You can also use the null-safe operator</t>
+  </si>
+  <si>
+    <t>&lt;div&gt;The current hero's name is {{game?.title}}&lt;/div&gt;
+&lt;div&gt;The null hero's name is {{game &amp;&amp; game.name}}&lt;/div&gt;</t>
+  </si>
+  <si>
+    <t>Template Expressions</t>
+  </si>
+  <si>
+    <t>The text between the curly brackets is evaluated to a string</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;The sum of two + two + four is {{2 + 2 + 4}}&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>Template expressions are not pure JavaScript</t>
+  </si>
+  <si>
+    <t>You cannot use these:</t>
+  </si>
+  <si>
+    <t>Assignments (=, +=, -=, ...)</t>
+  </si>
+  <si>
+    <t>The new operator</t>
+  </si>
+  <si>
+    <t>Multiple expressions</t>
+  </si>
+  <si>
+    <t>Increment or decrement operations (++ or --)</t>
+  </si>
+  <si>
+    <t>Bitwise operators</t>
+  </si>
+  <si>
+    <t>Types of Data Binding</t>
+  </si>
+  <si>
+    <t>There are three types of data binding</t>
+  </si>
+  <si>
+    <t>From data-source to view</t>
+  </si>
+  <si>
+    <t>{{expression}}
+[target]="expression"
+bind-target="expression"</t>
+  </si>
+  <si>
+    <t>From view to data-source</t>
+  </si>
+  <si>
+    <t>(target)="statement"
+on-target="statement"</t>
+  </si>
+  <si>
+    <t>Two-way</t>
+  </si>
+  <si>
+    <t>[(ngModel)]="expression"
+bindon-target="expression"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FormsModule needed
+</t>
+  </si>
+  <si>
+    <t>Lifecycle Hooks - Intersect Through the Loop</t>
+  </si>
+  <si>
+    <t>NgOnInit and NgOnDestroy Example</t>
+  </si>
+  <si>
+    <t>import { Component, OnInit, OnDestroy } from '@angular/core';
+@Component({..})
+export class GamesComponent implements OnInit, OnDestroy {
+  games: Game[];</t>
+  </si>
+  <si>
+    <t>ngOnInit() {
+   console.log('CREATED');
+  }</t>
+  </si>
+  <si>
+    <t>ngOnDestroy() {
+   console.log('DELETED');
+  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Called shortly after creation
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Used for cleanup
+</t>
+  </si>
+  <si>
+    <t>Other Lifecycle Hooks</t>
+  </si>
+  <si>
+    <t>ngOnChanges() - when data is changed</t>
+  </si>
+  <si>
+    <t>ngDoCheck() - detect your own changes</t>
+  </si>
+  <si>
+    <t>ngAfterContentInit() - when external content is received</t>
+  </si>
+  <si>
+    <t>ngAfterContentChecked() - when external content is checked</t>
+  </si>
+  <si>
+    <t>ngAfterViewInit() - when the views and child views are created</t>
+  </si>
+  <si>
+    <t>ngAfterViewChecked() - when the above are checked</t>
+  </si>
+  <si>
+    <t>More at: https://angular.io/guide/lifecycle-hooks</t>
+  </si>
+  <si>
+    <t>Component Interaction - Passing Data in Between</t>
+  </si>
+  <si>
+    <t>From Parent to Child</t>
+  </si>
+  <si>
+    <t>import { Component, Input } from '@angular/core';
+import { Game } from '../games/game';</t>
+  </si>
+  <si>
+    <t>"@Component({
+  selector: 'game',
+  template: `
+&lt;li&gt;&lt;div&gt;{{game.title | uppercase}}
+&lt;span *ngIf="game.price &gt;= 100"&gt;-&gt; Price: {{game.price}}&lt;/span&gt;
+&lt;/div&gt;&lt;/li&gt;`
+})"</t>
+  </si>
+  <si>
+    <t>export class GameComponent {
+  @Input('gameProp') game : Game;
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The prop will come from parent
+</t>
+  </si>
+  <si>
+    <t>&lt;h1&gt;Games List&lt;/h1&gt;
+ &lt;p&gt;Pick a game to Buy&lt;/p&gt;
+   &lt;ul&gt;
+ &lt;game *ngFor="let game of games" 
+   [gameProp]="game"&gt;
+ &lt;/game&gt;
+   &lt;/ul&gt;
+&lt;button (click)="showAdditionalContent()"&gt;Show Image&lt;/button&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Render the child into the parent template and pass the needed prop
+</t>
+  </si>
+  <si>
+    <t>In order to pass data from child to parent component we need the Output decorator and an Event Emitter</t>
+  </si>
+  <si>
+    <t>import { Output, EventEmitter } from '@angular/core'; export class GameComponent {
+ @Input('gameProp') game : Game;
+ @Output() onReacted = new EventEmitter&lt;boolean&gt;();
+  react(isLiked : boolean) {
+  this.onReacted.emit(isLiked); 
+ } 
+}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The parent will receive the event
+</t>
+  </si>
+  <si>
+    <t>The Parent component handles the event</t>
+  </si>
+  <si>
+    <t>&lt;game *ngFor="let game of games="[gameProp]"="game"      (onReacted)="onReacted($event)"&gt;
+&lt;/game&gt;</t>
+  </si>
+  <si>
+    <t>export class GamesComponent {
+ games: Game[];
+ likes: number;
+ dislikes : number;
+ onReacted(isLiked: boolean) {  
+  isLiked ? this.likes++ : this.dislikes++; 
+ }
+}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">&lt;button </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(click)="showContent($event)"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;Show Content&lt;/button&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>ng generate component</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>home</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>&lt;img [attr.src]="</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>imgUrl</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">" /&gt;
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -220,7 +936,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -230,6 +946,45 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -503,7 +1258,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -513,8 +1268,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,4 +1427,891 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D156"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="57.140625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="55" style="4" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+    </row>
+    <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" s="6"/>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="16" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="6"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B12" s="6"/>
+      <c r="C12" s="6"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
+    </row>
+    <row r="14" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="6"/>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16" s="6"/>
+      <c r="B16" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="B17" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" s="6"/>
+    </row>
+    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+    </row>
+    <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B19" s="6"/>
+      <c r="C19" s="6"/>
+    </row>
+    <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="6"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
+    </row>
+    <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C23" s="6"/>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C24" s="6"/>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="6"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C26" s="6"/>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="6"/>
+    </row>
+    <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+    </row>
+    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="10"/>
+      <c r="B30" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="10"/>
+      <c r="B31" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="10"/>
+      <c r="B32" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+    </row>
+    <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+    </row>
+    <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+    </row>
+    <row r="39" spans="1:3" ht="150" x14ac:dyDescent="0.25">
+      <c r="A39" s="11" t="s">
+        <v>151</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+    </row>
+    <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A41" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>153</v>
+      </c>
+      <c r="C41" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B42" s="3"/>
+      <c r="C42" s="3"/>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A44" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A45" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A46" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="12"/>
+      <c r="B53" s="4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="12"/>
+      <c r="B55" s="4" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="12"/>
+      <c r="B56" s="4" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="12"/>
+      <c r="B57" s="4" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B58" s="3"/>
+      <c r="C58" s="3"/>
+    </row>
+    <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B59" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="C59" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="D59" s="13"/>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="11"/>
+      <c r="B60" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="C60" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="D60" s="13"/>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="11"/>
+      <c r="B61" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="C61" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="D61" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B62" s="3"/>
+      <c r="C62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="12"/>
+      <c r="B65" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="12" t="s">
+        <v>129</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="12"/>
+      <c r="B67" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="12"/>
+      <c r="B68" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="12"/>
+      <c r="B69" s="4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="12"/>
+      <c r="B70" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="12"/>
+      <c r="B71" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="12"/>
+      <c r="B72" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B73" s="3"/>
+      <c r="C73" s="3"/>
+    </row>
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="15" t="s">
+        <v>138</v>
+      </c>
+      <c r="B74" s="4" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A75" s="15"/>
+      <c r="B75" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="15"/>
+      <c r="B76" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A78" s="14" t="s">
+        <v>145</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="C78" s="11" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A79" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A80" s="11"/>
+      <c r="B80" s="4" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="11"/>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="11"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="11"/>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="11"/>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="11"/>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="11"/>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="11"/>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="11"/>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="11"/>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="11"/>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="11"/>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="11"/>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="11"/>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="11"/>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="11"/>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="11"/>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="11"/>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="11"/>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="11"/>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="11"/>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="11"/>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="11"/>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="11"/>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="11"/>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="11"/>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="11"/>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="11"/>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="11"/>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="11"/>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="11"/>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="11"/>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="11"/>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="11"/>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A114" s="11"/>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A115" s="11"/>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A116" s="11"/>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A117" s="11"/>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A118" s="11"/>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A119" s="11"/>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A120" s="11"/>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A121" s="11"/>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" s="11"/>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" s="11"/>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A124" s="11"/>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" s="11"/>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A126" s="11"/>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A127" s="11"/>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A128" s="11"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="11"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="11"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="11"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="11"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="11"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="11"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="11"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="11"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="11"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="11"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="11"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="11"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="11"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="11"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="11"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="11"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="11"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="11"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="11"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="11"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="11"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="11"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="11"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="11"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="11"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="11"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="11"/>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A156" s="11"/>
+    </row>
+  </sheetData>
+  <mergeCells count="21">
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:A65"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A22:C22"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Angular - Components Complete
</commit_message>
<xml_diff>
--- a/Angular/Angular - ноември 2020/Angular.xlsx
+++ b/Angular/Angular - ноември 2020/Angular.xlsx
@@ -1,14 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="1.Angular-Introduction" sheetId="1" r:id="rId1"/>
-    <sheet name="02.Components" sheetId="2" r:id="rId2"/>
+    <sheet name="Commands" sheetId="3" r:id="rId1"/>
+    <sheet name="1.Angular-Introduction" sheetId="1" r:id="rId2"/>
+    <sheet name="02.Components" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
   <si>
     <t>tsc myfile.ts</t>
   </si>
@@ -870,17 +871,49 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Generate a new angular app</t>
+  </si>
+  <si>
+    <t>ng new articles-app</t>
+  </si>
+  <si>
+    <t>Start the app with the command</t>
+  </si>
+  <si>
+    <t>ng serve</t>
+  </si>
+  <si>
+    <t>ng generate component article</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate an article component with command </t>
+  </si>
+  <si>
+    <t>Command</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -909,8 +942,24 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -923,6 +972,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -933,19 +987,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -956,38 +1008,45 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1258,7 +1317,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1266,10 +1325,62 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="A1" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>159</v>
+      </c>
+      <c r="B4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1281,11 +1392,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1360,11 +1471,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="12"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1396,11 +1507,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1429,54 +1540,54 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="B75" sqref="B75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="57.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="50.42578125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="55" style="4" customWidth="1"/>
+    <col min="1" max="1" width="57.140625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="50.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="55" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="5"/>
+      <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="4" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>39</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -1484,811 +1595,823 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="7" t="s">
+      <c r="A5" s="16"/>
+      <c r="B5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="16"/>
+      <c r="B6" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="8"/>
-      <c r="B7" s="7" t="s">
+      <c r="A7" s="16"/>
+      <c r="B7" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="5"/>
+      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="6"/>
+      <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="C11" s="6"/>
+      <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="6" t="s">
+      <c r="A13" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
+      <c r="A15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="6"/>
+      <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="6"/>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="5"/>
+      <c r="B16" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="C16" s="9" t="s">
+      <c r="C16" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="6"/>
-      <c r="B17" s="6" t="s">
+      <c r="A17" s="5"/>
+      <c r="B17" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="6"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+      <c r="A18" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
+      <c r="B18" s="12"/>
+      <c r="C18" s="12"/>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
+      <c r="A20" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="C20" s="6"/>
+      <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
+      <c r="A21" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="12" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
+      <c r="B22" s="12"/>
+      <c r="C22" s="12"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="B23" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C24" s="6"/>
+      <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="A25" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="6"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="6" t="s">
+      <c r="A26" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C26" s="6"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
+      <c r="A27" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="B27" s="6"/>
-      <c r="C27" s="6"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="A28" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
     </row>
     <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="4" t="s">
+      <c r="B29" s="3" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="10"/>
-      <c r="B30" s="4" t="s">
+      <c r="A30" s="15"/>
+      <c r="B30" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="10"/>
-      <c r="B31" s="4" t="s">
+      <c r="A31" s="15"/>
+      <c r="B31" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="10"/>
-      <c r="B32" s="4" t="s">
+      <c r="A32" s="15"/>
+      <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="3" t="s">
+      <c r="A33" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
     </row>
     <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="4" t="s">
+      <c r="A34" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A35" s="4" t="s">
+      <c r="A35" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="11" t="s">
+      <c r="B35" s="8" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="3" t="s">
+      <c r="A36" s="12" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
+      <c r="B36" s="12"/>
+      <c r="C36" s="12"/>
     </row>
     <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
+      <c r="A37" s="3" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+      <c r="A38" s="12" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="3"/>
-      <c r="C38" s="3"/>
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
     </row>
     <row r="39" spans="1:3" ht="150" x14ac:dyDescent="0.25">
-      <c r="A39" s="11" t="s">
+      <c r="A39" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="B39" s="3" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
+      <c r="A40" s="12" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="12"/>
+      <c r="C40" s="12"/>
     </row>
     <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A41" s="4" t="s">
+      <c r="A41" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="C41" s="8" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
+      <c r="A42" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="3"/>
-      <c r="C42" s="3"/>
+      <c r="B42" s="12"/>
+      <c r="C42" s="12"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="B43" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="105" x14ac:dyDescent="0.25">
-      <c r="A44" s="11" t="s">
+      <c r="A44" s="8" t="s">
         <v>90</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B44" s="3" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A45" s="11" t="s">
+      <c r="A45" s="8" t="s">
         <v>94</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B45" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="90" x14ac:dyDescent="0.25">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A47" s="11" t="s">
+      <c r="A47" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="4" t="s">
+      <c r="B47" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="C47" s="8" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="11" t="s">
+      <c r="A48" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B48" s="3" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+      <c r="A49" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
+      <c r="B49" s="12"/>
+      <c r="C49" s="12"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="11" t="s">
+      <c r="A50" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B50" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="11" t="s">
+      <c r="A51" s="8" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="12" t="s">
+      <c r="A52" s="13" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="12"/>
-      <c r="B53" s="4" t="s">
+      <c r="A53" s="13"/>
+      <c r="B53" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="12"/>
-      <c r="B54" s="4" t="s">
+      <c r="A54" s="13"/>
+      <c r="B54" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="12"/>
-      <c r="B55" s="4" t="s">
+      <c r="A55" s="13"/>
+      <c r="B55" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="12"/>
-      <c r="B56" s="4" t="s">
+      <c r="A56" s="13"/>
+      <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="12"/>
-      <c r="B57" s="4" t="s">
+      <c r="A57" s="13"/>
+      <c r="B57" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="3" t="s">
+      <c r="A58" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="3"/>
-      <c r="C58" s="3"/>
+      <c r="B58" s="12"/>
+      <c r="C58" s="12"/>
     </row>
     <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="11" t="s">
+      <c r="A59" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="8" t="s">
         <v>115</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="8" t="s">
         <v>116</v>
       </c>
-      <c r="D59" s="13"/>
+      <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="11"/>
-      <c r="B60" s="11" t="s">
+      <c r="A60" s="8"/>
+      <c r="B60" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="D60" s="13"/>
+      <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="11"/>
-      <c r="B61" s="11" t="s">
+      <c r="A61" s="8"/>
+      <c r="B61" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="C61" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="8" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="3" t="s">
+      <c r="A62" s="12" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="3"/>
-      <c r="C62" s="3"/>
+      <c r="B62" s="12"/>
+      <c r="C62" s="12"/>
     </row>
     <row r="63" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="12" t="s">
+      <c r="A63" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="4" t="s">
+      <c r="B63" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="12"/>
-      <c r="B64" s="4" t="s">
+      <c r="A64" s="13"/>
+      <c r="B64" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="12"/>
-      <c r="B65" s="4" t="s">
+      <c r="A65" s="13"/>
+      <c r="B65" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C65" s="4" t="s">
+      <c r="C65" s="3" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="12" t="s">
+      <c r="A66" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="4" t="s">
+      <c r="B66" s="3" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="4" t="s">
+      <c r="A67" s="13"/>
+      <c r="B67" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="12"/>
-      <c r="B68" s="4" t="s">
+      <c r="A68" s="13"/>
+      <c r="B68" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="12"/>
-      <c r="B69" s="4" t="s">
+      <c r="A69" s="13"/>
+      <c r="B69" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="12"/>
-      <c r="B70" s="4" t="s">
+      <c r="A70" s="13"/>
+      <c r="B70" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="12"/>
-      <c r="B71" s="4" t="s">
+      <c r="A71" s="13"/>
+      <c r="B71" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="12"/>
-      <c r="B72" s="4" t="s">
+      <c r="A72" s="13"/>
+      <c r="B72" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
+      <c r="A73" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="B73" s="3"/>
-      <c r="C73" s="3"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
     </row>
     <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="15" t="s">
+      <c r="A74" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B74" s="3" t="s">
         <v>139</v>
       </c>
     </row>
     <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A75" s="15"/>
-      <c r="B75" s="4" t="s">
+      <c r="A75" s="14"/>
+      <c r="B75" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="15"/>
-      <c r="B76" s="4" t="s">
+      <c r="A76" s="14"/>
+      <c r="B76" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A77" s="15"/>
-      <c r="B77" s="4" t="s">
+      <c r="A77" s="14"/>
+      <c r="B77" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="C77" s="8" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A78" s="14" t="s">
+      <c r="A78" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="8" t="s">
         <v>146</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="C78" s="8" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A79" s="14" t="s">
+      <c r="A79" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="B79" s="4" t="s">
+      <c r="B79" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A80" s="11"/>
-      <c r="B80" s="4" t="s">
+      <c r="A80" s="8"/>
+      <c r="B80" s="3" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="11"/>
+      <c r="A81" s="8"/>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="11"/>
+      <c r="A82" s="8"/>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="11"/>
+      <c r="A83" s="8"/>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="11"/>
+      <c r="A84" s="8"/>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="11"/>
+      <c r="A85" s="8"/>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="11"/>
+      <c r="A86" s="8"/>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="11"/>
+      <c r="A87" s="8"/>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="11"/>
+      <c r="A88" s="8"/>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="11"/>
+      <c r="A89" s="8"/>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="11"/>
+      <c r="A90" s="8"/>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="11"/>
+      <c r="A91" s="8"/>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="11"/>
+      <c r="A92" s="8"/>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="11"/>
+      <c r="A93" s="8"/>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="11"/>
+      <c r="A94" s="8"/>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="11"/>
+      <c r="A95" s="8"/>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="11"/>
+      <c r="A96" s="8"/>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="11"/>
+      <c r="A97" s="8"/>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="11"/>
+      <c r="A98" s="8"/>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="11"/>
+      <c r="A99" s="8"/>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="11"/>
+      <c r="A100" s="8"/>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="11"/>
+      <c r="A101" s="8"/>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="11"/>
+      <c r="A102" s="8"/>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="11"/>
+      <c r="A103" s="8"/>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="11"/>
+      <c r="A104" s="8"/>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="11"/>
+      <c r="A105" s="8"/>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="11"/>
+      <c r="A106" s="8"/>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="11"/>
+      <c r="A107" s="8"/>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="11"/>
+      <c r="A108" s="8"/>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="11"/>
+      <c r="A109" s="8"/>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="11"/>
+      <c r="A110" s="8"/>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="11"/>
+      <c r="A111" s="8"/>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="11"/>
+      <c r="A112" s="8"/>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="11"/>
+      <c r="A113" s="8"/>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A114" s="11"/>
+      <c r="A114" s="8"/>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A115" s="11"/>
+      <c r="A115" s="8"/>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A116" s="11"/>
+      <c r="A116" s="8"/>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A117" s="11"/>
+      <c r="A117" s="8"/>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A118" s="11"/>
+      <c r="A118" s="8"/>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A119" s="11"/>
+      <c r="A119" s="8"/>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A120" s="11"/>
+      <c r="A120" s="8"/>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A121" s="11"/>
+      <c r="A121" s="8"/>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A122" s="11"/>
+      <c r="A122" s="8"/>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A123" s="11"/>
+      <c r="A123" s="8"/>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A124" s="11"/>
+      <c r="A124" s="8"/>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A125" s="11"/>
+      <c r="A125" s="8"/>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A126" s="11"/>
+      <c r="A126" s="8"/>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A127" s="11"/>
+      <c r="A127" s="8"/>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A128" s="11"/>
+      <c r="A128" s="8"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A129" s="11"/>
+      <c r="A129" s="8"/>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A130" s="11"/>
+      <c r="A130" s="8"/>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A131" s="11"/>
+      <c r="A131" s="8"/>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A132" s="11"/>
+      <c r="A132" s="8"/>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A133" s="11"/>
+      <c r="A133" s="8"/>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A134" s="11"/>
+      <c r="A134" s="8"/>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A135" s="11"/>
+      <c r="A135" s="8"/>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A136" s="11"/>
+      <c r="A136" s="8"/>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A137" s="11"/>
+      <c r="A137" s="8"/>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A138" s="11"/>
+      <c r="A138" s="8"/>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A139" s="11"/>
+      <c r="A139" s="8"/>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A140" s="11"/>
+      <c r="A140" s="8"/>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A141" s="11"/>
+      <c r="A141" s="8"/>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A142" s="11"/>
+      <c r="A142" s="8"/>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A143" s="11"/>
+      <c r="A143" s="8"/>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A144" s="11"/>
+      <c r="A144" s="8"/>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A145" s="11"/>
+      <c r="A145" s="8"/>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A146" s="11"/>
+      <c r="A146" s="8"/>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A147" s="11"/>
+      <c r="A147" s="8"/>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A148" s="11"/>
+      <c r="A148" s="8"/>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A149" s="11"/>
+      <c r="A149" s="8"/>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A150" s="11"/>
+      <c r="A150" s="8"/>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A151" s="11"/>
+      <c r="A151" s="8"/>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A152" s="11"/>
+      <c r="A152" s="8"/>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A153" s="11"/>
+      <c r="A153" s="8"/>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A154" s="11"/>
+      <c r="A154" s="8"/>
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A155" s="11"/>
+      <c r="A155" s="8"/>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A156" s="11"/>
+      <c r="A156" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A40:C40"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A18:C18"/>
+    <mergeCell ref="A22:C22"/>
+    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A36:C36"/>
+    <mergeCell ref="A38:C38"/>
     <mergeCell ref="A66:A72"/>
     <mergeCell ref="A73:C73"/>
     <mergeCell ref="A74:A77"/>
@@ -2298,18 +2421,6 @@
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="A62:C62"/>
     <mergeCell ref="A63:A65"/>
-    <mergeCell ref="A28:C28"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A36:C36"/>
-    <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A40:C40"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A10:C10"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A18:C18"/>
-    <mergeCell ref="A22:C22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Angular - DI, RXJX
</commit_message>
<xml_diff>
--- a/Angular/Angular - ноември 2020/Angular.xlsx
+++ b/Angular/Angular - ноември 2020/Angular.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="3" r:id="rId1"/>
     <sheet name="1.Angular-Introduction" sheetId="1" r:id="rId2"/>
     <sheet name="02.Components" sheetId="2" r:id="rId3"/>
+    <sheet name="3.DI, INTRO TO RXJS, SERVICES" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="145621"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="321">
   <si>
     <t>tsc myfile.ts</t>
   </si>
@@ -895,17 +896,916 @@
   <si>
     <t>Description</t>
   </si>
+  <si>
+    <t>Mobile Apps</t>
+  </si>
+  <si>
+    <t>https://ionicframework.com/</t>
+  </si>
+  <si>
+    <t>SOLID Principles. RxJS. Services</t>
+  </si>
+  <si>
+    <t>Change Detection Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angular performs change detection on all components (from top to bottom) every time something changes
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change detection is very performant, but as an app gets more complex and the amount of components grows, change detection will have to perform more and more work
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The strategy that the default change detector uses to detect changes
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">enum ChangeDetectionStrategy {
+  OnPush: 0,
+  Default: 1
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">When set, takes effect the next time change detection is triggered
+</t>
+  </si>
+  <si>
+    <t>Change Detection Strategy - Members</t>
+  </si>
+  <si>
+    <t>Automatic change detection is deactivated until reactivated by setting the strategy to Default</t>
+  </si>
+  <si>
+    <t>This strategy applies to all child directives and cannot be overridden</t>
+  </si>
+  <si>
+    <t>Default: 1 - CheckAlways strategy</t>
+  </si>
+  <si>
+    <t>OnPush: 0 - CheckOne strategy</t>
+  </si>
+  <si>
+    <t>Use the default CheckAlways strategy</t>
+  </si>
+  <si>
+    <t>Change detection is automatic until explicitly deactivated</t>
+  </si>
+  <si>
+    <t>SOLID Principles</t>
+  </si>
+  <si>
+    <t>Single Responsibility Principle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The responsibility should be entirely encapsulated by the class
+</t>
+  </si>
+  <si>
+    <t>A responsibility can be defined as a reason to change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Every class should have only one responsibility </t>
+  </si>
+  <si>
+    <t xml:space="preserve">This principle leads to
+</t>
+  </si>
+  <si>
+    <t>Stronger cohesion and looser coupling</t>
+  </si>
+  <si>
+    <t>Better readability</t>
+  </si>
+  <si>
+    <t>Lower complexity</t>
+  </si>
+  <si>
+    <t>Open-Closed Principle</t>
+  </si>
+  <si>
+    <t>Adding new behavior doesn't require changes  over existing source code</t>
+  </si>
+  <si>
+    <t>Closed for modification</t>
+  </si>
+  <si>
+    <t>Open for extension</t>
+  </si>
+  <si>
+    <t>Software entities like classes, modules and functions should be open for extension, but closed for                            modification</t>
+  </si>
+  <si>
+    <t>Changing the source code is not allowed</t>
+  </si>
+  <si>
+    <t>Liskov Substitution Principle</t>
+  </si>
+  <si>
+    <t>Derived types must be completely substitutable for their base types</t>
+  </si>
+  <si>
+    <t>Derived classes</t>
+  </si>
+  <si>
+    <t>Must not remove base class behavior</t>
+  </si>
+  <si>
+    <t>Only extend functionalities of the base class</t>
+  </si>
+  <si>
+    <t>Interface Segregation Principle</t>
+  </si>
+  <si>
+    <t>It is better to have many smaller interfaces, than fewer, fatter ones</t>
+  </si>
+  <si>
+    <t>"Fat" interfaces need to be divided into "role" interfaces (small and more specific)</t>
+  </si>
+  <si>
+    <t>Classes that implement interfaces, should not be forced to implement methods they do not use</t>
+  </si>
+  <si>
+    <t>Dependency Inversion Principle</t>
+  </si>
+  <si>
+    <t>High-level modules should not depend on low-level modules. Both should depend on abstractions</t>
+  </si>
+  <si>
+    <t>Abstractions should not depend on details. Details should depend on abstractions</t>
+  </si>
+  <si>
+    <t>The design principle does not just change the direction of the dependency</t>
+  </si>
+  <si>
+    <t>Splits the dependency between the high-level and low-level</t>
+  </si>
+  <si>
+    <t>The high-level module depends on the abstraction</t>
+  </si>
+  <si>
+    <t>The low-level depends on the same abstraction</t>
+  </si>
+  <si>
+    <t>Dependency is another object that your class needs</t>
+  </si>
+  <si>
+    <t>Examples (Framework, Database, File System, Providers)</t>
+  </si>
+  <si>
+    <t>Dependency Injection - Apply for Depependency Inversion</t>
+  </si>
+  <si>
+    <t>Classes that dependent on each other are called  coupled</t>
+  </si>
+  <si>
+    <t>Dependencies are bad because they decrease reuse</t>
+  </si>
+  <si>
+    <t>public class Customer {
+  customerService = new CustomerService('Service');}</t>
+  </si>
+  <si>
+    <t>Customer class is dependent on concrete service</t>
+  </si>
+  <si>
+    <t>Dependency Injection is a popular design pattern</t>
+  </si>
+  <si>
+    <t>Inversion of Control (IoC)</t>
+  </si>
+  <si>
+    <t>Dependencies are pushed in the class from the outside</t>
+  </si>
+  <si>
+    <t>The class does not instantiate it's dependencies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The service(CustomerService) comes from outside
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class Customer {
+  private customerService;
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  constructor(cService: CustomerService)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {
+    this.customerService = cService;
+}}</t>
+    </r>
+  </si>
+  <si>
+    <t>Classic Violations</t>
+  </si>
+  <si>
+    <t>Using the new keyword</t>
+  </si>
+  <si>
+    <t>Using static methods/properties</t>
+  </si>
+  <si>
+    <t>public class Laptop {
+  public battery: Battery;
+  public videoCard: VideoCard;
+  constructor() {
+    this.battery = new Battery('Acer battery');
+    this.videoCard = new VideoCard('Nvidia 960 GTX');
+  }}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The class is brittle, inflexible and hard to test
+</t>
+  </si>
+  <si>
+    <t>Add the dependencies through the constructor</t>
+  </si>
+  <si>
+    <t>constructor(
+ public videoCard: VideoCard, 
+ public battery: Battery)</t>
+  </si>
+  <si>
+    <t>Create whatever model you like</t>
+  </si>
+  <si>
+    <t>let firstLaptop = new Laptop(   new VideoCard('Nvidia 940m'),    new Battery('Acer Battery'));</t>
+  </si>
+  <si>
+    <t xml:space="preserve">let secondLaptop = new Laptop(   new VideoCard('Radeon 280x'), 
+  new Battery('Toshiba Battery'));
+</t>
+  </si>
+  <si>
+    <t>General Requirements</t>
+  </si>
+  <si>
+    <t>https://angular.io/guide/dependency-injection-pattern</t>
+  </si>
+  <si>
+    <t>A class should receive its dependencies from external sources rather than creating them itself</t>
+  </si>
+  <si>
+    <t>Decouple dependencies through constructor injection</t>
+  </si>
+  <si>
+    <t>Your code should be easier to test</t>
+  </si>
+  <si>
+    <t>Additional information</t>
+  </si>
+  <si>
+    <t>Services - Constructor Injection, Providers, Injectable</t>
+  </si>
+  <si>
+    <t>Why We Need Services?</t>
+  </si>
+  <si>
+    <t>Components shouldn't fetch or save data directly</t>
+  </si>
+  <si>
+    <t>They should focus on presenting data and delegate data access to a service</t>
+  </si>
+  <si>
+    <t>Services are a great way to</t>
+  </si>
+  <si>
+    <t>Share information among classes that don't know about each other</t>
+  </si>
+  <si>
+    <t>Avoid code duplication</t>
+  </si>
+  <si>
+    <t>Services in Angular are just normal TypeScript classes that  handle data manipulation</t>
+  </si>
+  <si>
+    <t>export class BooksService {
+  booksData: Book[];
+  addBook(b: Book) {
+    this.booksData.push(b);
+  }}</t>
+  </si>
+  <si>
+    <t>Services are injected into components via constructor injection</t>
+  </si>
+  <si>
+    <t>Before that they should be provided from inside the decorator</t>
+  </si>
+  <si>
+    <t>The same instance will be provided for child components</t>
+  </si>
+  <si>
+    <t>In order to inject one service into another use the  @Injectable decorator</t>
+  </si>
+  <si>
+    <t>"@Injectable()
+export class BooksService {
+  booksData: Book[];
+  constructor (
+    private loggingService: LoggingService
+  ) { }}"</t>
+  </si>
+  <si>
+    <t>"@Component({
+  providers: [ BooksService ]
+})
+export class BookListComponent {
+  constructor(
+    private booksService: BooksService
+  ) {  }}"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">"@Injectable({ providedIn: 'root' })" - Provided in 'app.module.ts'
+</t>
+  </si>
+  <si>
+    <t>RxJS and Observables</t>
+  </si>
+  <si>
+    <t>The Observable</t>
+  </si>
+  <si>
+    <t>In Angular we handle streams using Observables</t>
+  </si>
+  <si>
+    <t>Create Streams</t>
+  </si>
+  <si>
+    <t>Subscribe to Streams</t>
+  </si>
+  <si>
+    <t>React to new values</t>
+  </si>
+  <si>
+    <t>Combine streams to build new ones</t>
+  </si>
+  <si>
+    <t>FRP is a paradigm for software development</t>
+  </si>
+  <si>
+    <t>Function Reactive Programming</t>
+  </si>
+  <si>
+    <t>Entire programs can be build uniquely around the notion of streams</t>
+  </si>
+  <si>
+    <t>Create, combine and subscribe to streams</t>
+  </si>
+  <si>
+    <t>The core goal of FRP</t>
+  </si>
+  <si>
+    <t>Build programs in a declarative way</t>
+  </si>
+  <si>
+    <t>Lack of application state variables</t>
+  </si>
+  <si>
+    <t>Introducing RxJS - Stands for Reactive Extensions for JavaScript</t>
+  </si>
+  <si>
+    <t>Install Library</t>
+  </si>
+  <si>
+    <t>npm install rxjs</t>
+  </si>
+  <si>
+    <t>RxJS - Reactive Extensions for JavaScript - Install Library</t>
+  </si>
+  <si>
+    <t>Use with CommonJS</t>
+  </si>
+  <si>
+    <t>const { range } = require('rxjs')
+const { map, filter } = require('rxjs/operators')</t>
+  </si>
+  <si>
+    <t>Use with import/export</t>
+  </si>
+  <si>
+    <t>import { range } from 'rxjs'
+import { map, filter } from 'rxjs/operators'</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Using the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tap</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operator</t>
+    </r>
+  </si>
+  <si>
+    <t>const obs = range(1, 10)
+  .pipe(
+    tap(i =&gt; console.log(`Hello: ${i}`))
+  );</t>
+  </si>
+  <si>
+    <t>Has no subscribers (cold)</t>
+  </si>
+  <si>
+    <t>Observables are either hot or cold</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">We need to subscribe to them:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>obs.subscribe(i =&gt; console.log(i));</t>
+    </r>
+  </si>
+  <si>
+    <t>Has a subscriber (hot)</t>
+  </si>
+  <si>
+    <t>Observables Side Effect (Hot vs Cold)</t>
+  </si>
+  <si>
+    <t>Observables are not shared by default</t>
+  </si>
+  <si>
+    <t>Creating a subscriber sets up a whole new separate processing  chain: 
+obs.subscribe(i =&gt; console.log(`first sub ${i}`));
+obs.subscribe(i =&gt; console.log(`second sub ${i}`));</t>
+  </si>
+  <si>
+    <t>Two things to keep in mind:</t>
+  </si>
+  <si>
+    <t>Is the observable hot or cold?</t>
+  </si>
+  <si>
+    <t>Is the observable shared or not?</t>
+  </si>
+  <si>
+    <t>Commonly Used RxJS Operators</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>map</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>filter</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> operator</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">reduce </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>operator</t>
+    </r>
+  </si>
+  <si>
+    <t>const obs = range(1, 10).pipe(map(i =&gt; i ** 2));</t>
+  </si>
+  <si>
+    <t>const obs = range(1, 10).pipe(filter(i =&gt; i % 2 === 0));</t>
+  </si>
+  <si>
+    <t>const obs = range(1, 10).pipe(
+  reduce((prevVal, val) =&gt; prevVal + val, 0)
+))</t>
+  </si>
+  <si>
+    <t>RxJS and FRP Overview</t>
+  </si>
+  <si>
+    <t>RxJS and FRP are powerful concepts</t>
+  </si>
+  <si>
+    <t>Multiple choice to structure an Angular app</t>
+  </si>
+  <si>
+    <t>Go full reactive (extensive use of RxJS)</t>
+  </si>
+  <si>
+    <t>Via parts (Forms or Http)</t>
+  </si>
+  <si>
+    <t>More on observables here: Click</t>
+  </si>
+  <si>
+    <t>More RxJS operators here: Click</t>
+  </si>
+  <si>
+    <t>HTTP Client - Fetching Data from a Remote API</t>
+  </si>
+  <si>
+    <t>Before using the HttpClient to fetch data, import the  HttpClientModule in "app.module.ts"</t>
+  </si>
+  <si>
+    <t>import { HttpClientModule } from '@angular/common/http'</t>
+  </si>
+  <si>
+    <t>Add the module in imports array</t>
+  </si>
+  <si>
+    <t>"@NgModule({
+declarations:[ // App Components ],
+imports:[ 
+   BrowserModule, 
+   HttpClientModule
+],"</t>
+  </si>
+  <si>
+    <t>From now on HttpClient can be injected in Services</t>
+  </si>
+  <si>
+    <t>Using the HTTP Client in Services</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Inject the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HttpClient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and use it as a service
+The </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Client</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> works with </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>generic</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> types
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">"@Injectable()
+export class PostsService {   constructor( 
+    private http : </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>HttpClient</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  
+  ) { }
+  getAllPosts() : Observable&lt;Post[]&gt; { 
+    const url = 'https://jsonplaceholder.typicode.com/posts';
+    return this.http.get</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;Post[]&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(url);
+  }
+}"</t>
+    </r>
+  </si>
+  <si>
+    <t>Inject a service and subscribe to observables</t>
+  </si>
+  <si>
+    <t>Always subscribe to observables</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">export class PostsComponent implements OnInit {
+  posts: Posts[];   constructor(
+   private postsService : PostsService
+  ) { }
+   ngOnInit(): void {
+   this.postsService.getAllPosts()
+      .subscribe(data =&gt; {
+        </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> this.posts </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>= data;
+      });
+  } }</t>
+    </r>
+  </si>
+  <si>
+    <t>Subscribe to the Observable</t>
+  </si>
+  <si>
+    <t>Type Checking the Response</t>
+  </si>
+  <si>
+    <t>It is recommended to cast the response</t>
+  </si>
+  <si>
+    <r>
+      <t>getAllPosts() : Observable&lt;Post[]&gt; { 
+ const url = 'https://jsonplaceholder.typicode.com/posts';
+ return this.http.get&lt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Post[]</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&gt;(url);
+}</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Should be an interface:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interface Post</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> {
+  userId: number;
+  id: number;
+  title: string;
+  body: string;
+}</t>
+    </r>
+  </si>
+  <si>
+    <t>To handle errors add an error handler to subscribe call</t>
+  </si>
+  <si>
+    <t>ngOnInit(): void {
+this.postsService.getAllPosts()
+  .subscribe(
+    data =&gt; { // Attach data to prop },
+    err =&gt; {
+      console.log(`${JSON.stringify(err)}`) 
+    }
+  )
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -958,8 +1858,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -977,6 +1885,12 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -987,16 +1901,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1008,7 +1923,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1020,33 +1935,50 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="4" readingOrder="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1317,7 +2249,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1325,10 +2257,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1338,35 +2270,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="15" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="13"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="14" t="s">
         <v>154</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B3" s="13" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
         <v>156</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B4" s="13" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B5" t="s">
         <v>158</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>270</v>
       </c>
     </row>
   </sheetData>
@@ -1377,10 +2321,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1392,11 +2336,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -1471,11 +2415,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="12"/>
+      <c r="B9" s="16"/>
+      <c r="C9" s="16"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -1507,11 +2451,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -1529,11 +2473,24 @@
         <v>14</v>
       </c>
     </row>
+    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A17" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="B17" s="16"/>
+      <c r="C17" s="16"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="12" t="s">
+        <v>163</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A9:C9"/>
     <mergeCell ref="A14:C14"/>
+    <mergeCell ref="A17:C17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1544,8 +2501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A73" sqref="A73:C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1557,11 +2514,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="12"/>
-      <c r="C1" s="12"/>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1584,7 +2541,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="17" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -1595,7 +2552,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="16"/>
+      <c r="A5" s="17"/>
       <c r="B5" s="6" t="s">
         <v>40</v>
       </c>
@@ -1604,7 +2561,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
+      <c r="A6" s="17"/>
       <c r="B6" s="6" t="s">
         <v>42</v>
       </c>
@@ -1613,7 +2570,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="16"/>
+      <c r="A7" s="17"/>
       <c r="B7" s="6" t="s">
         <v>44</v>
       </c>
@@ -1636,11 +2593,11 @@
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
+      <c r="B10" s="16"/>
+      <c r="C10" s="16"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -1666,11 +2623,11 @@
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="12" t="s">
+      <c r="A14" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
+      <c r="B14" s="16"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -1698,11 +2655,11 @@
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16"/>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -1728,11 +2685,11 @@
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="12"/>
-      <c r="C22" s="12"/>
+      <c r="B22" s="16"/>
+      <c r="C22" s="16"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -1778,14 +2735,14 @@
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="12" t="s">
+      <c r="A28" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="12"/>
-      <c r="C28" s="12"/>
+      <c r="B28" s="16"/>
+      <c r="C28" s="16"/>
     </row>
     <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="15" t="s">
+      <c r="A29" s="18" t="s">
         <v>77</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1793,29 +2750,29 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="15"/>
+      <c r="A30" s="18"/>
       <c r="B30" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="15"/>
+      <c r="A31" s="18"/>
       <c r="B31" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="15"/>
+      <c r="A32" s="18"/>
       <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
+      <c r="B33" s="16"/>
+      <c r="C33" s="16"/>
     </row>
     <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -1831,11 +2788,11 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="12" t="s">
+      <c r="A36" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="12"/>
-      <c r="C36" s="12"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="16"/>
     </row>
     <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -1843,11 +2800,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="12" t="s">
+      <c r="A38" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="12"/>
-      <c r="C38" s="12"/>
+      <c r="B38" s="16"/>
+      <c r="C38" s="16"/>
     </row>
     <row r="39" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
@@ -1858,11 +2815,11 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="12" t="s">
+      <c r="A40" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
+      <c r="B40" s="16"/>
+      <c r="C40" s="16"/>
     </row>
     <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -1876,11 +2833,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="12" t="s">
+      <c r="A42" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="B42" s="16"/>
+      <c r="C42" s="16"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -1934,11 +2891,11 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="12" t="s">
+      <c r="A49" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="12"/>
-      <c r="C49" s="12"/>
+      <c r="B49" s="16"/>
+      <c r="C49" s="16"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
@@ -1954,46 +2911,46 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="A52" s="19" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="13"/>
+      <c r="A53" s="19"/>
       <c r="B53" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="13"/>
+      <c r="A54" s="19"/>
       <c r="B54" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="13"/>
+      <c r="A55" s="19"/>
       <c r="B55" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="13"/>
+      <c r="A56" s="19"/>
       <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="13"/>
+      <c r="A57" s="19"/>
       <c r="B57" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="12" t="s">
+      <c r="A58" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="12"/>
-      <c r="C58" s="12"/>
+      <c r="B58" s="16"/>
+      <c r="C58" s="16"/>
     </row>
     <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
@@ -2030,14 +2987,14 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="12" t="s">
+      <c r="A62" s="16" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="12"/>
-      <c r="C62" s="12"/>
+      <c r="B62" s="16"/>
+      <c r="C62" s="16"/>
     </row>
     <row r="63" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="13" t="s">
+      <c r="A63" s="19" t="s">
         <v>123</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -2045,7 +3002,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="13"/>
+      <c r="A64" s="19"/>
       <c r="B64" s="3" t="s">
         <v>125</v>
       </c>
@@ -2054,7 +3011,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="13"/>
+      <c r="A65" s="19"/>
       <c r="B65" s="3" t="s">
         <v>126</v>
       </c>
@@ -2063,7 +3020,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="13" t="s">
+      <c r="A66" s="19" t="s">
         <v>129</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -2071,50 +3028,50 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
+      <c r="A67" s="19"/>
       <c r="B67" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="13"/>
+      <c r="A68" s="19"/>
       <c r="B68" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="13"/>
+      <c r="A69" s="19"/>
       <c r="B69" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="13"/>
+      <c r="A70" s="19"/>
       <c r="B70" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="13"/>
+      <c r="A71" s="19"/>
       <c r="B71" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="13"/>
+      <c r="A72" s="19"/>
       <c r="B72" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="12" t="s">
+      <c r="A73" s="16" t="s">
         <v>137</v>
       </c>
-      <c r="B73" s="12"/>
-      <c r="C73" s="12"/>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
     </row>
     <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="14" t="s">
+      <c r="A74" s="20" t="s">
         <v>138</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -2122,13 +3079,13 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A75" s="14"/>
+      <c r="A75" s="20"/>
       <c r="B75" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="14"/>
+      <c r="A76" s="20"/>
       <c r="B76" s="3" t="s">
         <v>141</v>
       </c>
@@ -2137,7 +3094,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A77" s="14"/>
+      <c r="A77" s="20"/>
       <c r="B77" s="3" t="s">
         <v>143</v>
       </c>
@@ -2400,6 +3357,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:A65"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:A7"/>
@@ -2412,17 +3378,1214 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A52:A57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A63:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D168"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="A106" sqref="A106:C106"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="41.140625" customWidth="1"/>
+    <col min="2" max="2" width="45.42578125" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" customWidth="1"/>
+    <col min="4" max="4" width="28.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>164</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+    </row>
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+    </row>
+    <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="16" t="s">
+        <v>171</v>
+      </c>
+      <c r="B7" s="16"/>
+      <c r="C7" s="16"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="B8" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="B10" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>179</v>
+      </c>
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="8"/>
+      <c r="B14" s="8" t="s">
+        <v>181</v>
+      </c>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
+      <c r="B15" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
+      <c r="B16" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="8" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="B19" s="21"/>
+      <c r="C19" s="21"/>
+    </row>
+    <row r="20" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+    </row>
+    <row r="21" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>190</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="C21" s="8"/>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="B23" s="21"/>
+      <c r="C23" s="21"/>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>194</v>
+      </c>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>197</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="19"/>
+      <c r="B26" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>198</v>
+      </c>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+    </row>
+    <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+    </row>
+    <row r="29" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>199</v>
+      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="8"/>
+    </row>
+    <row r="31" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A31" s="21" t="s">
+        <v>202</v>
+      </c>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+    </row>
+    <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A32" s="8" t="s">
+        <v>203</v>
+      </c>
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="B34" s="8"/>
+      <c r="C34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="19"/>
+      <c r="B36" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="C36" s="8"/>
+    </row>
+    <row r="37" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A37" s="21" t="s">
+        <v>211</v>
+      </c>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+    </row>
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>209</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="C38" s="8"/>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B39" s="8"/>
+      <c r="C39" s="8"/>
+    </row>
+    <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>214</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="B41" s="8"/>
+      <c r="C41" s="8"/>
+    </row>
+    <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="19"/>
+      <c r="B43" s="8" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
+    </row>
+    <row r="44" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+    </row>
+    <row r="46" spans="1:4" ht="135" x14ac:dyDescent="0.25">
+      <c r="A46" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="C47" s="8"/>
+    </row>
+    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="8" t="s">
+        <v>229</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="21" t="s">
+        <v>232</v>
+      </c>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+    </row>
+    <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B50" s="8"/>
+      <c r="C50" s="8"/>
+    </row>
+    <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B51" s="8"/>
+      <c r="C51" s="8"/>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="B52" s="8"/>
+      <c r="C52" s="8"/>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B53" s="8"/>
+      <c r="C53" s="8"/>
+    </row>
+    <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="B54" s="8"/>
+      <c r="C54" s="8"/>
+    </row>
+    <row r="55" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A55" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="B55" s="16"/>
+      <c r="C55" s="16"/>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="C56" s="8"/>
+    </row>
+    <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
+      <c r="B57" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C57" s="8"/>
+    </row>
+    <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
+      <c r="B58" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="8"/>
+      <c r="B59" s="8"/>
+      <c r="C59" s="8" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A60" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>246</v>
+      </c>
+      <c r="C60" s="8"/>
+    </row>
+    <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B61" s="8"/>
+      <c r="C61" s="8"/>
+    </row>
+    <row r="62" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A62" s="8" t="s">
+        <v>248</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="C62" s="8" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="8" t="s">
+        <v>250</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C63" s="8" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="B64" s="16"/>
+      <c r="C64" s="16"/>
+    </row>
+    <row r="65" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="B65" s="21"/>
+      <c r="C65" s="21"/>
+    </row>
+    <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A66" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="C66" s="8"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="8"/>
+      <c r="B67" s="8" t="s">
+        <v>258</v>
+      </c>
+      <c r="C67" s="8"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="8"/>
+      <c r="B68" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C68" s="8"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="8"/>
+      <c r="B69" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="21" t="s">
+        <v>262</v>
+      </c>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+    </row>
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="19" t="s">
+        <v>261</v>
+      </c>
+      <c r="B71" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="19"/>
+      <c r="B72" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="C72" s="8"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="B73" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C73" s="8"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="8"/>
+      <c r="B74" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="21" t="s">
+        <v>268</v>
+      </c>
+      <c r="B75" s="21"/>
+      <c r="C75" s="21"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="B76" s="8" t="s">
+        <v>270</v>
+      </c>
+      <c r="C76" s="8"/>
+    </row>
+    <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>272</v>
+      </c>
+      <c r="B77" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="C77" s="8"/>
+    </row>
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>274</v>
+      </c>
+      <c r="B78" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="C78" s="8"/>
+    </row>
+    <row r="79" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A79" s="21" t="s">
+        <v>282</v>
+      </c>
+      <c r="B79" s="21"/>
+      <c r="C79" s="21"/>
+    </row>
+    <row r="80" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A80" s="8" t="s">
+        <v>276</v>
+      </c>
+      <c r="B80" s="8" t="s">
+        <v>277</v>
+      </c>
+      <c r="C80" s="8" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A81" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="B81" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="C81" s="8" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A82" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B82" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="C82" s="8"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="B83" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C83" s="8"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="8"/>
+      <c r="B84" s="8" t="s">
+        <v>287</v>
+      </c>
+      <c r="C84" s="8"/>
+    </row>
+    <row r="85" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A85" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="B85" s="21"/>
+      <c r="C85" s="21"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="B86" s="8" t="s">
+        <v>292</v>
+      </c>
+      <c r="C86" s="8"/>
+    </row>
+    <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="B87" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C87" s="8"/>
+    </row>
+    <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A88" s="8" t="s">
+        <v>291</v>
+      </c>
+      <c r="B88" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="C88" s="8"/>
+    </row>
+    <row r="89" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A89" s="21" t="s">
+        <v>295</v>
+      </c>
+      <c r="B89" s="21"/>
+      <c r="C89" s="21"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="B90" s="8"/>
+      <c r="C90" s="8"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="B91" s="8" t="s">
+        <v>298</v>
+      </c>
+      <c r="C91" s="8"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="19"/>
+      <c r="B92" s="8" t="s">
+        <v>299</v>
+      </c>
+      <c r="C92" s="8"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="25" t="s">
+        <v>300</v>
+      </c>
+      <c r="B93" s="8"/>
+      <c r="C93" s="8"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="25" t="s">
+        <v>301</v>
+      </c>
+      <c r="B94" s="8"/>
+      <c r="C94" s="8"/>
+    </row>
+    <row r="95" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A95" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="B95" s="16"/>
+      <c r="C95" s="16"/>
+    </row>
+    <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A96" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="B96" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="C96" s="8"/>
+    </row>
+    <row r="97" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="A97" s="8" t="s">
+        <v>305</v>
+      </c>
+      <c r="B97" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="C97" s="8" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="21" t="s">
+        <v>308</v>
+      </c>
+      <c r="B98" s="21"/>
+      <c r="C98" s="21"/>
+    </row>
+    <row r="99" spans="1:3" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="23" t="s">
+        <v>310</v>
+      </c>
+      <c r="B99" s="23"/>
+      <c r="C99" s="8" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="21" t="s">
+        <v>314</v>
+      </c>
+      <c r="B100" s="21"/>
+      <c r="C100" s="21"/>
+    </row>
+    <row r="101" spans="1:3" ht="165" x14ac:dyDescent="0.25">
+      <c r="A101" s="8" t="s">
+        <v>311</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>313</v>
+      </c>
+      <c r="C101" s="8" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A102" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="B102" s="21"/>
+      <c r="C102" s="21"/>
+    </row>
+    <row r="103" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A103" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="B103" s="8" t="s">
+        <v>317</v>
+      </c>
+      <c r="C103" s="8" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A104" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="B104" s="21"/>
+      <c r="C104" s="21"/>
+    </row>
+    <row r="105" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A105" s="8" t="s">
+        <v>319</v>
+      </c>
+      <c r="B105" s="8" t="s">
+        <v>320</v>
+      </c>
+      <c r="C105" s="8"/>
+    </row>
+    <row r="106" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A106" s="16"/>
+      <c r="B106" s="16"/>
+      <c r="C106" s="16"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="8"/>
+      <c r="B107" s="8"/>
+      <c r="C107" s="8"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="8"/>
+      <c r="B108" s="8"/>
+      <c r="C108" s="8"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="8"/>
+      <c r="B109" s="8"/>
+      <c r="C109" s="8"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="8"/>
+      <c r="B110" s="8"/>
+      <c r="C110" s="8"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="8"/>
+      <c r="B111" s="8"/>
+      <c r="C111" s="8"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A112" s="8"/>
+      <c r="B112" s="8"/>
+      <c r="C112" s="8"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A113" s="8"/>
+      <c r="B113" s="8"/>
+      <c r="C113" s="8"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A114" s="8"/>
+      <c r="B114" s="8"/>
+      <c r="C114" s="8"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A115" s="8"/>
+      <c r="B115" s="8"/>
+      <c r="C115" s="8"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A116" s="8"/>
+      <c r="B116" s="8"/>
+      <c r="C116" s="8"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A117" s="8"/>
+      <c r="B117" s="8"/>
+      <c r="C117" s="8"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A118" s="8"/>
+      <c r="B118" s="8"/>
+      <c r="C118" s="8"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A119" s="8"/>
+      <c r="B119" s="8"/>
+      <c r="C119" s="8"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A120" s="8"/>
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A121" s="8"/>
+      <c r="B121" s="8"/>
+      <c r="C121" s="8"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A122" s="8"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A123" s="8"/>
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A124" s="8"/>
+      <c r="B124" s="8"/>
+      <c r="C124" s="8"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A125" s="8"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="8"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A126" s="8"/>
+      <c r="B126" s="8"/>
+      <c r="C126" s="8"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A127" s="8"/>
+      <c r="B127" s="8"/>
+      <c r="C127" s="8"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A128" s="8"/>
+      <c r="B128" s="8"/>
+      <c r="C128" s="8"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A129" s="8"/>
+      <c r="B129" s="8"/>
+      <c r="C129" s="8"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A130" s="8"/>
+      <c r="B130" s="8"/>
+      <c r="C130" s="8"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A131" s="8"/>
+      <c r="B131" s="8"/>
+      <c r="C131" s="8"/>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A132" s="8"/>
+      <c r="B132" s="8"/>
+      <c r="C132" s="8"/>
+    </row>
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A133" s="8"/>
+      <c r="B133" s="8"/>
+      <c r="C133" s="8"/>
+    </row>
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A134" s="8"/>
+      <c r="B134" s="8"/>
+      <c r="C134" s="8"/>
+    </row>
+    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A135" s="8"/>
+      <c r="B135" s="8"/>
+      <c r="C135" s="8"/>
+    </row>
+    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A136" s="8"/>
+      <c r="B136" s="8"/>
+      <c r="C136" s="8"/>
+    </row>
+    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A137" s="8"/>
+      <c r="B137" s="8"/>
+      <c r="C137" s="8"/>
+    </row>
+    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A138" s="8"/>
+      <c r="B138" s="8"/>
+      <c r="C138" s="8"/>
+    </row>
+    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A139" s="8"/>
+      <c r="B139" s="8"/>
+      <c r="C139" s="8"/>
+    </row>
+    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A140" s="8"/>
+      <c r="B140" s="8"/>
+      <c r="C140" s="8"/>
+    </row>
+    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A141" s="8"/>
+      <c r="B141" s="8"/>
+      <c r="C141" s="8"/>
+    </row>
+    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A142" s="8"/>
+      <c r="B142" s="8"/>
+      <c r="C142" s="8"/>
+    </row>
+    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A143" s="8"/>
+      <c r="B143" s="8"/>
+      <c r="C143" s="8"/>
+    </row>
+    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A144" s="8"/>
+      <c r="B144" s="8"/>
+      <c r="C144" s="8"/>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A145" s="8"/>
+      <c r="B145" s="8"/>
+      <c r="C145" s="8"/>
+    </row>
+    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A146" s="8"/>
+      <c r="B146" s="8"/>
+      <c r="C146" s="8"/>
+    </row>
+    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A147" s="8"/>
+      <c r="B147" s="8"/>
+      <c r="C147" s="8"/>
+    </row>
+    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A148" s="8"/>
+      <c r="B148" s="8"/>
+      <c r="C148" s="8"/>
+    </row>
+    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A149" s="8"/>
+      <c r="B149" s="8"/>
+      <c r="C149" s="8"/>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A150" s="8"/>
+      <c r="B150" s="8"/>
+      <c r="C150" s="8"/>
+    </row>
+    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A151" s="8"/>
+      <c r="B151" s="8"/>
+      <c r="C151" s="8"/>
+    </row>
+    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A152" s="8"/>
+      <c r="B152" s="8"/>
+      <c r="C152" s="8"/>
+    </row>
+    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A153" s="8"/>
+      <c r="B153" s="8"/>
+      <c r="C153" s="8"/>
+    </row>
+    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A154" s="8"/>
+      <c r="B154" s="8"/>
+      <c r="C154" s="8"/>
+    </row>
+    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A155" s="8"/>
+      <c r="B155" s="8"/>
+      <c r="C155" s="8"/>
+    </row>
+    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A156" s="8"/>
+      <c r="B156" s="8"/>
+      <c r="C156" s="8"/>
+    </row>
+    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A157" s="8"/>
+      <c r="B157" s="8"/>
+      <c r="C157" s="8"/>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A158" s="8"/>
+      <c r="B158" s="8"/>
+      <c r="C158" s="8"/>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A159" s="8"/>
+      <c r="B159" s="8"/>
+      <c r="C159" s="8"/>
+    </row>
+    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A160" s="8"/>
+      <c r="B160" s="8"/>
+      <c r="C160" s="8"/>
+    </row>
+    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A161" s="8"/>
+      <c r="B161" s="8"/>
+      <c r="C161" s="8"/>
+    </row>
+    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A162" s="8"/>
+      <c r="B162" s="8"/>
+      <c r="C162" s="8"/>
+    </row>
+    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A163" s="8"/>
+      <c r="B163" s="8"/>
+      <c r="C163" s="8"/>
+    </row>
+    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A164" s="8"/>
+      <c r="B164" s="8"/>
+      <c r="C164" s="8"/>
+    </row>
+    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A165" s="8"/>
+      <c r="B165" s="8"/>
+      <c r="C165" s="8"/>
+    </row>
+    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A166" s="8"/>
+      <c r="B166" s="8"/>
+      <c r="C166" s="8"/>
+    </row>
+    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A167" s="8"/>
+      <c r="B167" s="8"/>
+      <c r="C167" s="8"/>
+    </row>
+    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A168" s="8"/>
+      <c r="B168" s="8"/>
+      <c r="C168" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="35">
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A95:C95"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A44:C44"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A93" r:id="rId1" display="https://blog.angular-university.io/functional-reactive-programming-for-angular-2-developers-rxjs-and-observables/"/>
+    <hyperlink ref="A94" r:id="rId2" display="http://reactivex.io/rxjs/class/es6/Observable.js~Observable.html"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Angular - WorkShop 1 Complete
</commit_message>
<xml_diff>
--- a/Angular/Angular - ноември 2020/Angular.xlsx
+++ b/Angular/Angular - ноември 2020/Angular.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
-  <workbookPr filterPrivacy="1"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="335">
   <si>
     <t>tsc myfile.ts</t>
   </si>
@@ -1796,17 +1796,60 @@
   <si>
     <t>Install angular</t>
   </si>
+  <si>
+    <t>Mongo</t>
+  </si>
+  <si>
+    <t>.\mongod</t>
+  </si>
+  <si>
+    <t>.\mongorestore.exe -d forum 'C:\Users\Admin\source\repos\Course\SoftUni\Angular\Angular - ноември 2020\WORKSHOP COMPONENTS\resources\forum'</t>
+  </si>
+  <si>
+    <t>restore database</t>
+  </si>
+  <si>
+    <t>start mongo</t>
+  </si>
+  <si>
+    <t>.\mongo.exe 
+use forum
+db.themes.find()</t>
+  </si>
+  <si>
+    <t>start shell and check database</t>
+  </si>
+  <si>
+    <t>ng genereate service user</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Generate a user service with command </t>
+  </si>
+  <si>
+    <t>Angular Language Service</t>
+  </si>
+  <si>
+    <t>Plugins &amp; Extensions</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1884,7 +1927,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1908,6 +1951,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1920,15 +1969,15 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1940,7 +1989,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1952,47 +2001,52 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2267,7 +2321,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2275,19 +2329,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="43.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
         <v>161</v>
       </c>
@@ -2295,15 +2351,15 @@
         <v>160</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>323</v>
       </c>
-      <c r="B2" s="26" t="s">
+      <c r="B2" s="28" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
         <v>321</v>
       </c>
@@ -2311,23 +2367,23 @@
         <v>322</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="28" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="18" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
         <v>159</v>
       </c>
@@ -2335,19 +2391,69 @@
         <v>158</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="13" t="s">
+        <v>332</v>
+      </c>
+      <c r="B7" s="28" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
         <v>271</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B8" s="15" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13"/>
-      <c r="B8" s="17"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="13"/>
+      <c r="B9" s="17"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>324</v>
+      </c>
+      <c r="B10" t="s">
+        <v>325</v>
+      </c>
+      <c r="C10" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="27"/>
+      <c r="B11" t="s">
+        <v>326</v>
+      </c>
+      <c r="C11" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="27"/>
+      <c r="B12" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C12" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="29" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>333</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A10:A12"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2357,8 +2463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2370,11 +2476,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2449,11 +2555,11 @@
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
@@ -2485,11 +2591,11 @@
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -2508,11 +2614,11 @@
       </c>
     </row>
     <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="B17" s="18"/>
-      <c r="C17" s="18"/>
+      <c r="B17" s="19"/>
+      <c r="C17" s="19"/>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
@@ -2535,8 +2641,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="A73" sqref="A73:C73"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2548,11 +2654,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2575,7 +2681,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="22" t="s">
         <v>37</v>
       </c>
       <c r="B4" s="6" t="s">
@@ -2586,7 +2692,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
+      <c r="A5" s="22"/>
       <c r="B5" s="6" t="s">
         <v>40</v>
       </c>
@@ -2595,7 +2701,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="6" t="s">
         <v>42</v>
       </c>
@@ -2604,7 +2710,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="6" t="s">
         <v>44</v>
       </c>
@@ -2627,11 +2733,11 @@
       <c r="C9" s="5"/>
     </row>
     <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
@@ -2657,11 +2763,11 @@
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="B14" s="18"/>
-      <c r="C14" s="18"/>
+      <c r="B14" s="19"/>
+      <c r="C14" s="19"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -2689,11 +2795,11 @@
       <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B18" s="18"/>
-      <c r="C18" s="18"/>
+      <c r="B18" s="19"/>
+      <c r="C18" s="19"/>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
@@ -2719,11 +2825,11 @@
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="B22" s="18"/>
-      <c r="C22" s="18"/>
+      <c r="B22" s="19"/>
+      <c r="C22" s="19"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
@@ -2769,14 +2875,14 @@
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="18"/>
-      <c r="C28" s="18"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
     </row>
     <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="20" t="s">
+      <c r="A29" s="23" t="s">
         <v>77</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -2784,29 +2890,29 @@
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="20"/>
+      <c r="A30" s="23"/>
       <c r="B30" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="20"/>
+      <c r="A31" s="23"/>
       <c r="B31" s="3" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="20"/>
+      <c r="A32" s="23"/>
       <c r="B32" s="3" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="18" t="s">
+      <c r="A33" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="B33" s="18"/>
-      <c r="C33" s="18"/>
+      <c r="B33" s="19"/>
+      <c r="C33" s="19"/>
     </row>
     <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
@@ -2822,11 +2928,11 @@
       </c>
     </row>
     <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="18" t="s">
+      <c r="A36" s="19" t="s">
         <v>82</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="18"/>
+      <c r="B36" s="19"/>
+      <c r="C36" s="19"/>
     </row>
     <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
@@ -2834,11 +2940,11 @@
       </c>
     </row>
     <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="18" t="s">
+      <c r="A38" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="18"/>
-      <c r="C38" s="18"/>
+      <c r="B38" s="19"/>
+      <c r="C38" s="19"/>
     </row>
     <row r="39" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
@@ -2849,11 +2955,11 @@
       </c>
     </row>
     <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="18" t="s">
+      <c r="A40" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="B40" s="18"/>
-      <c r="C40" s="18"/>
+      <c r="B40" s="19"/>
+      <c r="C40" s="19"/>
     </row>
     <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
@@ -2867,11 +2973,11 @@
       </c>
     </row>
     <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="B42" s="18"/>
-      <c r="C42" s="18"/>
+      <c r="B42" s="19"/>
+      <c r="C42" s="19"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
@@ -2925,11 +3031,11 @@
       </c>
     </row>
     <row r="49" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="B49" s="18"/>
-      <c r="C49" s="18"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="19"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
@@ -2945,46 +3051,46 @@
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="21" t="s">
+      <c r="A52" s="20" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="21"/>
+      <c r="A53" s="20"/>
       <c r="B53" s="3" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="21"/>
+      <c r="A54" s="20"/>
       <c r="B54" s="3" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="21"/>
+      <c r="A55" s="20"/>
       <c r="B55" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="21"/>
+      <c r="A56" s="20"/>
       <c r="B56" s="3" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="21"/>
+      <c r="A57" s="20"/>
       <c r="B57" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="B58" s="18"/>
-      <c r="C58" s="18"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="19"/>
     </row>
     <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
@@ -3021,14 +3127,14 @@
       </c>
     </row>
     <row r="62" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="19" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="18"/>
-      <c r="C62" s="18"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="19"/>
     </row>
     <row r="63" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="21" t="s">
+      <c r="A63" s="20" t="s">
         <v>123</v>
       </c>
       <c r="B63" s="3" t="s">
@@ -3036,7 +3142,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="21"/>
+      <c r="A64" s="20"/>
       <c r="B64" s="3" t="s">
         <v>125</v>
       </c>
@@ -3045,7 +3151,7 @@
       </c>
     </row>
     <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="21"/>
+      <c r="A65" s="20"/>
       <c r="B65" s="3" t="s">
         <v>126</v>
       </c>
@@ -3054,7 +3160,7 @@
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="21" t="s">
+      <c r="A66" s="20" t="s">
         <v>129</v>
       </c>
       <c r="B66" s="3" t="s">
@@ -3062,50 +3168,50 @@
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="21"/>
+      <c r="A67" s="20"/>
       <c r="B67" s="3" t="s">
         <v>131</v>
       </c>
     </row>
     <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="21"/>
+      <c r="A68" s="20"/>
       <c r="B68" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="21"/>
+      <c r="A69" s="20"/>
       <c r="B69" s="3" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="21"/>
+      <c r="A70" s="20"/>
       <c r="B70" s="3" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="21"/>
+      <c r="A71" s="20"/>
       <c r="B71" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="21"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="3" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="18" t="s">
+      <c r="A73" s="19" t="s">
         <v>137</v>
       </c>
-      <c r="B73" s="18"/>
-      <c r="C73" s="18"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="19"/>
     </row>
     <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="22" t="s">
+      <c r="A74" s="21" t="s">
         <v>138</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -3113,13 +3219,13 @@
       </c>
     </row>
     <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A75" s="22"/>
+      <c r="A75" s="21"/>
       <c r="B75" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="22"/>
+      <c r="A76" s="21"/>
       <c r="B76" s="3" t="s">
         <v>141</v>
       </c>
@@ -3128,7 +3234,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A77" s="22"/>
+      <c r="A77" s="21"/>
       <c r="B77" s="3" t="s">
         <v>143</v>
       </c>
@@ -3391,15 +3497,6 @@
     </row>
   </sheetData>
   <mergeCells count="21">
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A52:A57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A63:A65"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:A7"/>
@@ -3412,6 +3509,15 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A38:C38"/>
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3422,8 +3528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D168"/>
   <sheetViews>
-    <sheetView topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="A106" sqref="A106:C106"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3435,18 +3541,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
     </row>
     <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
@@ -3472,11 +3578,11 @@
       </c>
     </row>
     <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="19" t="s">
         <v>171</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="18"/>
+      <c r="B7" s="19"/>
+      <c r="C7" s="19"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -3505,18 +3611,18 @@
       </c>
     </row>
     <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="18"/>
-      <c r="C12" s="18"/>
+      <c r="B12" s="19"/>
+      <c r="C12" s="19"/>
     </row>
     <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="24" t="s">
         <v>179</v>
       </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
@@ -3536,7 +3642,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="20" t="s">
         <v>183</v>
       </c>
       <c r="C16" s="8" t="s">
@@ -3545,24 +3651,24 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="21"/>
+      <c r="B17" s="20"/>
       <c r="C17" s="8" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
-      <c r="B18" s="21"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="8" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="23" t="s">
+      <c r="A19" s="24" t="s">
         <v>187</v>
       </c>
-      <c r="B19" s="23"/>
-      <c r="C19" s="23"/>
+      <c r="B19" s="24"/>
+      <c r="C19" s="24"/>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
@@ -3590,11 +3696,11 @@
       <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="23" t="s">
+      <c r="A23" s="24" t="s">
         <v>193</v>
       </c>
-      <c r="B23" s="23"/>
-      <c r="C23" s="23"/>
+      <c r="B23" s="24"/>
+      <c r="C23" s="24"/>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
@@ -3604,7 +3710,7 @@
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
+      <c r="A25" s="20" t="s">
         <v>195</v>
       </c>
       <c r="B25" s="8" t="s">
@@ -3613,18 +3719,18 @@
       <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="21"/>
+      <c r="A26" s="20"/>
       <c r="B26" s="8" t="s">
         <v>196</v>
       </c>
       <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="23" t="s">
+      <c r="A27" s="24" t="s">
         <v>198</v>
       </c>
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
     </row>
     <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
@@ -3648,11 +3754,11 @@
       <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="23" t="s">
+      <c r="A31" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="B31" s="23"/>
-      <c r="C31" s="23"/>
+      <c r="B31" s="24"/>
+      <c r="C31" s="24"/>
     </row>
     <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
@@ -3676,7 +3782,7 @@
       <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="20" t="s">
         <v>206</v>
       </c>
       <c r="B35" s="8" t="s">
@@ -3685,18 +3791,18 @@
       <c r="C35" s="8"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="21"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="8" t="s">
         <v>208</v>
       </c>
       <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="23" t="s">
+      <c r="A37" s="24" t="s">
         <v>211</v>
       </c>
-      <c r="B37" s="23"/>
-      <c r="C37" s="23"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
@@ -3733,13 +3839,13 @@
       <c r="C41" s="8"/>
     </row>
     <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="21" t="s">
+      <c r="A42" s="20" t="s">
         <v>217</v>
       </c>
       <c r="B42" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C42" s="24" t="s">
+      <c r="C42" s="26" t="s">
         <v>221</v>
       </c>
       <c r="D42" s="25" t="s">
@@ -3747,19 +3853,19 @@
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="21"/>
+      <c r="A43" s="20"/>
       <c r="B43" s="8" t="s">
         <v>219</v>
       </c>
-      <c r="C43" s="24"/>
+      <c r="C43" s="26"/>
       <c r="D43" s="25"/>
     </row>
     <row r="44" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="23" t="s">
+      <c r="A44" s="24" t="s">
         <v>222</v>
       </c>
-      <c r="B44" s="23"/>
-      <c r="C44" s="23"/>
+      <c r="B44" s="24"/>
+      <c r="C44" s="24"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
@@ -3800,11 +3906,11 @@
       </c>
     </row>
     <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="23" t="s">
+      <c r="A49" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="B49" s="23"/>
-      <c r="C49" s="23"/>
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
     </row>
     <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
@@ -3842,11 +3948,11 @@
       <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="19" t="s">
         <v>238</v>
       </c>
-      <c r="B55" s="18"/>
-      <c r="C55" s="18"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="19"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
@@ -3919,18 +4025,18 @@
       </c>
     </row>
     <row r="64" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="19" t="s">
         <v>254</v>
       </c>
-      <c r="B64" s="18"/>
-      <c r="C64" s="18"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="19"/>
     </row>
     <row r="65" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
+      <c r="A65" s="24" t="s">
         <v>255</v>
       </c>
-      <c r="B65" s="23"/>
-      <c r="C65" s="23"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
     </row>
     <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
@@ -3963,14 +4069,14 @@
       <c r="C69" s="8"/>
     </row>
     <row r="70" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="24" t="s">
         <v>262</v>
       </c>
-      <c r="B70" s="23"/>
-      <c r="C70" s="23"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
     </row>
     <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="21" t="s">
+      <c r="A71" s="20" t="s">
         <v>261</v>
       </c>
       <c r="B71" s="8" t="s">
@@ -3979,7 +4085,7 @@
       <c r="C71" s="8"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="21"/>
+      <c r="A72" s="20"/>
       <c r="B72" s="8" t="s">
         <v>264</v>
       </c>
@@ -4002,11 +4108,11 @@
       <c r="C74" s="8"/>
     </row>
     <row r="75" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="24" t="s">
         <v>268</v>
       </c>
-      <c r="B75" s="23"/>
-      <c r="C75" s="23"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
@@ -4036,11 +4142,11 @@
       <c r="C78" s="8"/>
     </row>
     <row r="79" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="24" t="s">
         <v>282</v>
       </c>
-      <c r="B79" s="23"/>
-      <c r="C79" s="23"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
     </row>
     <row r="80" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
@@ -4090,11 +4196,11 @@
       <c r="C84" s="8"/>
     </row>
     <row r="85" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="23" t="s">
+      <c r="A85" s="24" t="s">
         <v>288</v>
       </c>
-      <c r="B85" s="23"/>
-      <c r="C85" s="23"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
@@ -4124,11 +4230,11 @@
       <c r="C88" s="8"/>
     </row>
     <row r="89" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A89" s="23" t="s">
+      <c r="A89" s="24" t="s">
         <v>295</v>
       </c>
-      <c r="B89" s="23"/>
-      <c r="C89" s="23"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
@@ -4138,7 +4244,7 @@
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="21" t="s">
+      <c r="A91" s="20" t="s">
         <v>297</v>
       </c>
       <c r="B91" s="8" t="s">
@@ -4147,7 +4253,7 @@
       <c r="C91" s="8"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="21"/>
+      <c r="A92" s="20"/>
       <c r="B92" s="8" t="s">
         <v>299</v>
       </c>
@@ -4168,11 +4274,11 @@
       <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="18" t="s">
+      <c r="A95" s="19" t="s">
         <v>302</v>
       </c>
-      <c r="B95" s="18"/>
-      <c r="C95" s="18"/>
+      <c r="B95" s="19"/>
+      <c r="C95" s="19"/>
     </row>
     <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
@@ -4195,11 +4301,11 @@
       </c>
     </row>
     <row r="98" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A98" s="23" t="s">
+      <c r="A98" s="24" t="s">
         <v>308</v>
       </c>
-      <c r="B98" s="23"/>
-      <c r="C98" s="23"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
     </row>
     <row r="99" spans="1:3" ht="195" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99" s="25" t="s">
@@ -4211,11 +4317,11 @@
       </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="23" t="s">
+      <c r="A100" s="24" t="s">
         <v>314</v>
       </c>
-      <c r="B100" s="23"/>
-      <c r="C100" s="23"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
     </row>
     <row r="101" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
@@ -4229,11 +4335,11 @@
       </c>
     </row>
     <row r="102" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A102" s="23" t="s">
+      <c r="A102" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="B102" s="23"/>
-      <c r="C102" s="23"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
     </row>
     <row r="103" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
@@ -4247,11 +4353,11 @@
       </c>
     </row>
     <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A104" s="23" t="s">
+      <c r="A104" s="24" t="s">
         <v>315</v>
       </c>
-      <c r="B104" s="23"/>
-      <c r="C104" s="23"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
     </row>
     <row r="105" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
@@ -4263,9 +4369,9 @@
       <c r="C105" s="8"/>
     </row>
     <row r="106" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A106" s="18"/>
-      <c r="B106" s="18"/>
-      <c r="C106" s="18"/>
+      <c r="A106" s="19"/>
+      <c r="B106" s="19"/>
+      <c r="C106" s="19"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
@@ -4579,12 +4685,23 @@
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="A106:C106"/>
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A102:C102"/>
-    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A7:C7"/>
+    <mergeCell ref="A12:C12"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="A23:C23"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:C27"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="A95:C95"/>
     <mergeCell ref="A49:C49"/>
     <mergeCell ref="A55:C55"/>
@@ -4597,23 +4714,12 @@
     <mergeCell ref="A85:C85"/>
     <mergeCell ref="A89:C89"/>
     <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A7:C7"/>
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="A23:C23"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:C27"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A104:C104"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A93" r:id="rId1" display="https://blog.angular-university.io/functional-reactive-programming-for-angular-2-developers-rxjs-and-observables/"/>

</xml_diff>

<commit_message>
Angular - Intro 2
</commit_message>
<xml_diff>
--- a/Angular/Angular - ноември 2020/Angular.xlsx
+++ b/Angular/Angular - ноември 2020/Angular.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Commands" sheetId="3" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="335">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="339">
   <si>
     <t>tsc myfile.ts</t>
   </si>
@@ -144,9 +144,6 @@
   </si>
   <si>
     <t>https://github.com/DefinitelyTyped/DefinitelyTyped</t>
-  </si>
-  <si>
-    <t>Дефиниции за TypeScript</t>
   </si>
   <si>
     <t>.\node_modules\.bin\tsc index.ts</t>
@@ -1831,17 +1828,79 @@
   <si>
     <t>Plugins &amp; Extensions</t>
   </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Generate </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>package.json</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> for holding dependencies</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">npm install @types/node --save-dev </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Дефиниции за Node.
+За  да сработи показването на методите във функциите с точка в tsconfig.json трябва да се резкоментира </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>types["node"]</t>
+    </r>
+  </si>
+  <si>
+    <t>Автоматичен компилатор за typescript</t>
+  </si>
+  <si>
+    <t>tsc --watch</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1969,15 +2028,15 @@
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1989,7 +2048,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2001,52 +2060,55 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="2" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="4" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2321,7 +2383,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2332,7 +2394,7 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+      <selection activeCell="A28" sqref="A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,66 +2407,66 @@
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="14" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
-        <v>323</v>
-      </c>
-      <c r="B2" s="28" t="s">
+        <v>322</v>
+      </c>
+      <c r="B2" s="20" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>320</v>
+      </c>
+      <c r="B3" s="17" t="s">
         <v>321</v>
-      </c>
-      <c r="B3" s="17" t="s">
-        <v>322</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
+        <v>153</v>
+      </c>
+      <c r="B4" s="20" t="s">
         <v>154</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="B5" s="18" t="s">
         <v>156</v>
-      </c>
-      <c r="B5" s="18" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="13" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B6" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="13" t="s">
-        <v>332</v>
-      </c>
-      <c r="B7" s="28" t="s">
         <v>331</v>
+      </c>
+      <c r="B7" s="20" t="s">
+        <v>330</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -2412,42 +2474,42 @@
       <c r="B9" s="17"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="27" t="s">
+      <c r="A10" s="22" t="s">
+        <v>323</v>
+      </c>
+      <c r="B10" t="s">
         <v>324</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="22"/>
+      <c r="B11" t="s">
         <v>325</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C11" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="22"/>
+      <c r="B12" s="3" t="s">
         <v>328</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="27"/>
-      <c r="B11" t="s">
-        <v>326</v>
-      </c>
-      <c r="C11" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="27"/>
-      <c r="B12" s="3" t="s">
+      <c r="C12" t="s">
         <v>329</v>
       </c>
-      <c r="C12" t="s">
-        <v>330</v>
-      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
-        <v>334</v>
+      <c r="A13" s="21" t="s">
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -2461,10 +2523,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2476,49 +2538,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>25</v>
+      <c r="C2" s="1" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="19" t="s">
         <v>21</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>20</v>
-      </c>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="19"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -2531,106 +2597,118 @@
         <v>2</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>27</v>
+        <v>336</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="19" t="s">
+        <v>337</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>338</v>
+      </c>
+      <c r="C9" s="19"/>
+    </row>
+    <row r="10" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="19"/>
-      <c r="C9" s="19"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+    <row r="15" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A15" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
-    </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>12</v>
-      </c>
+      <c r="B15" s="23"/>
+      <c r="C15" s="23"/>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
+        <v>161</v>
+      </c>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="12" t="s">
         <v>162</v>
-      </c>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="12" t="s">
-        <v>163</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="A1:C1"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A17:C17"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="A15:C15"/>
+    <mergeCell ref="A18:C18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2641,7 +2719,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D156"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B76" sqref="B76"/>
     </sheetView>
   </sheetViews>
@@ -2654,617 +2732,617 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
+      <c r="A1" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
     </row>
     <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C2" s="4"/>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="4" t="s">
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="24" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="6" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="24"/>
+      <c r="B5" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="24"/>
+      <c r="B6" s="6" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="C6" s="4" t="s">
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="24"/>
+      <c r="B7" s="6" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="6" t="s">
-        <v>44</v>
       </c>
       <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
     </row>
     <row r="9" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B9" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="C9" s="5"/>
+    </row>
+    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="C9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="19"/>
-      <c r="C10" s="19"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="23"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C11" s="5"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
     </row>
     <row r="14" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B14" s="19"/>
-      <c r="C14" s="19"/>
+      <c r="A14" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="B14" s="23"/>
+      <c r="C14" s="23"/>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="C15" s="5"/>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5"/>
       <c r="B17" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="5"/>
+    </row>
+    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A18" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="C17" s="5"/>
-    </row>
-    <row r="18" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="19"/>
-      <c r="C18" s="19"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="23"/>
     </row>
     <row r="19" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B19" s="5"/>
       <c r="C19" s="5"/>
     </row>
     <row r="20" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>60</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>61</v>
       </c>
       <c r="C20" s="5"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B21" s="5"/>
       <c r="C21" s="5"/>
     </row>
     <row r="22" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B22" s="19"/>
-      <c r="C22" s="19"/>
+      <c r="A22" s="23" t="s">
+        <v>57</v>
+      </c>
+      <c r="B22" s="23"/>
+      <c r="C22" s="23"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="C23" s="5"/>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="5" t="s">
         <v>65</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>66</v>
       </c>
       <c r="C24" s="5"/>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B25" s="5" t="s">
         <v>67</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>68</v>
       </c>
       <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B27" s="5"/>
       <c r="C27" s="5"/>
     </row>
     <row r="28" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A28" s="19" t="s">
+      <c r="A28" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" s="23"/>
+      <c r="C28" s="23"/>
+    </row>
+    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="25"/>
+      <c r="B30" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B28" s="19"/>
-      <c r="C28" s="19"/>
-    </row>
-    <row r="29" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="23" t="s">
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="25"/>
+      <c r="B31" s="3" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="25"/>
+      <c r="B32" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A33" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="23"/>
-      <c r="B30" s="3" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="23"/>
-      <c r="B31" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="23"/>
-      <c r="B32" s="3" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A33" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="B33" s="19"/>
-      <c r="C33" s="19"/>
+      <c r="B33" s="23"/>
+      <c r="C33" s="23"/>
     </row>
     <row r="34" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="B35" s="8" t="s">
+    </row>
+    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A36" s="23" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A36" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
+      <c r="B36" s="23"/>
+      <c r="C36" s="23"/>
     </row>
     <row r="37" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A38" s="23" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A38" s="19" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="19"/>
-      <c r="C38" s="19"/>
+      <c r="B38" s="23"/>
+      <c r="C38" s="23"/>
     </row>
     <row r="39" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B39" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A40" s="23" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A40" s="19" t="s">
-        <v>86</v>
-      </c>
-      <c r="B40" s="19"/>
-      <c r="C40" s="19"/>
+      <c r="B40" s="23"/>
+      <c r="C40" s="23"/>
     </row>
     <row r="41" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>152</v>
+      </c>
+      <c r="C41" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>153</v>
-      </c>
-      <c r="C41" s="8" t="s">
+    </row>
+    <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A42" s="23" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="B42" s="19"/>
-      <c r="C42" s="19"/>
+      <c r="B42" s="23"/>
+      <c r="C42" s="23"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B43" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B43" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="B45" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B46" s="3" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="47" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="8" t="s">
         <v>99</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B48" s="3" t="s">
+    </row>
+    <row r="49" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="23" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
-        <v>103</v>
-      </c>
-      <c r="B49" s="19"/>
-      <c r="C49" s="19"/>
+      <c r="B49" s="23"/>
+      <c r="C49" s="23"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>104</v>
-      </c>
-      <c r="B50" s="3" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="26" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="20" t="s">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="26"/>
+      <c r="B53" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="20"/>
-      <c r="B53" s="3" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="26"/>
+      <c r="B54" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="3" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="26"/>
+      <c r="B55" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="3" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="26"/>
+      <c r="B56" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="20"/>
-      <c r="B56" s="3" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="26"/>
+      <c r="B57" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="20"/>
-      <c r="B57" s="3" t="s">
+    <row r="58" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A58" s="23" t="s">
         <v>112</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
-        <v>113</v>
-      </c>
-      <c r="B58" s="19"/>
-      <c r="C58" s="19"/>
+      <c r="B58" s="23"/>
+      <c r="C58" s="23"/>
     </row>
     <row r="59" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B59" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="B59" s="8" t="s">
+      <c r="C59" s="8" t="s">
         <v>115</v>
-      </c>
-      <c r="C59" s="8" t="s">
-        <v>116</v>
       </c>
       <c r="D59" s="9"/>
     </row>
     <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="8"/>
       <c r="B60" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="C60" s="8" t="s">
         <v>117</v>
-      </c>
-      <c r="C60" s="8" t="s">
-        <v>118</v>
       </c>
       <c r="D60" s="9"/>
     </row>
     <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="8"/>
       <c r="B61" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C61" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="C61" s="8" t="s">
+      <c r="D61" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="D61" s="8" t="s">
+    </row>
+    <row r="62" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A62" s="23" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="B62" s="23"/>
+      <c r="C62" s="23"/>
+    </row>
+    <row r="63" spans="1:4" ht="105" x14ac:dyDescent="0.25">
+      <c r="A63" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="B62" s="19"/>
-      <c r="C62" s="19"/>
-    </row>
-    <row r="63" spans="1:4" ht="105" x14ac:dyDescent="0.25">
-      <c r="A63" s="20" t="s">
+      <c r="B63" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B63" s="3" t="s">
+    </row>
+    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A64" s="26"/>
+      <c r="B64" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
-      <c r="B64" s="3" t="s">
+      <c r="C64" s="3" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A65" s="26"/>
+      <c r="B65" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="C64" s="3" t="s">
+      <c r="C65" s="3" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="20"/>
-      <c r="B65" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="C65" s="3" t="s">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="26" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="20" t="s">
+      <c r="B66" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="3" t="s">
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="26"/>
+      <c r="B67" s="3" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="20"/>
-      <c r="B67" s="3" t="s">
+    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A68" s="26"/>
+      <c r="B68" s="3" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="68" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
-      <c r="B68" s="3" t="s">
+    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A69" s="26"/>
+      <c r="B69" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="69" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="3" t="s">
+    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A70" s="26"/>
+      <c r="B70" s="3" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="70" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="3" t="s">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="26"/>
+      <c r="B71" s="3" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
-      <c r="B71" s="3" t="s">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="26"/>
+      <c r="B72" s="3" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="3" t="s">
+    <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A73" s="23" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="73" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="B73" s="23"/>
+      <c r="C73" s="23"/>
+    </row>
+    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="B73" s="19"/>
-      <c r="C73" s="19"/>
-    </row>
-    <row r="74" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A74" s="21" t="s">
+      <c r="B74" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B74" s="3" t="s">
+    </row>
+    <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+      <c r="A75" s="27"/>
+      <c r="B75" s="3" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="75" spans="1:3" ht="120" x14ac:dyDescent="0.25">
-      <c r="A75" s="21"/>
-      <c r="B75" s="3" t="s">
+    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="27"/>
+      <c r="B76" s="3" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="21"/>
-      <c r="B76" s="3" t="s">
+      <c r="C76" s="3" t="s">
         <v>141</v>
       </c>
-      <c r="C76" s="3" t="s">
+    </row>
+    <row r="77" spans="1:3" ht="135" x14ac:dyDescent="0.25">
+      <c r="A77" s="27"/>
+      <c r="B77" s="3" t="s">
         <v>142</v>
       </c>
-    </row>
-    <row r="77" spans="1:3" ht="135" x14ac:dyDescent="0.25">
-      <c r="A77" s="21"/>
-      <c r="B77" s="3" t="s">
+      <c r="C77" s="8" t="s">
         <v>143</v>
-      </c>
-      <c r="C77" s="8" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="78" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A78" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B78" s="8" t="s">
         <v>145</v>
       </c>
-      <c r="B78" s="8" t="s">
+      <c r="C78" s="8" t="s">
         <v>146</v>
-      </c>
-      <c r="C78" s="8" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="79" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A79" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B79" s="3" t="s">
         <v>148</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="80" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.25">
@@ -3497,6 +3575,15 @@
     </row>
   </sheetData>
   <mergeCells count="21">
+    <mergeCell ref="A66:A72"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="A74:A77"/>
+    <mergeCell ref="A42:C42"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A52:A57"/>
+    <mergeCell ref="A58:C58"/>
+    <mergeCell ref="A62:C62"/>
+    <mergeCell ref="A63:A65"/>
     <mergeCell ref="A40:C40"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A4:A7"/>
@@ -3509,15 +3596,6 @@
     <mergeCell ref="A33:C33"/>
     <mergeCell ref="A36:C36"/>
     <mergeCell ref="A38:C38"/>
-    <mergeCell ref="A66:A72"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="A74:A77"/>
-    <mergeCell ref="A42:C42"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A52:A57"/>
-    <mergeCell ref="A58:C58"/>
-    <mergeCell ref="A62:C62"/>
-    <mergeCell ref="A63:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -3541,837 +3619,837 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A2" s="23" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="19"/>
-      <c r="C1" s="19"/>
-    </row>
-    <row r="2" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="19" t="s">
-        <v>165</v>
-      </c>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>168</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A7" s="23" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
-        <v>171</v>
-      </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="19"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B8" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B10" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="23" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="19" t="s">
+      <c r="B12" s="23"/>
+      <c r="C12" s="23"/>
+    </row>
+    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A13" s="28" t="s">
         <v>178</v>
       </c>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-    </row>
-    <row r="13" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>179</v>
-      </c>
-      <c r="B13" s="24"/>
-      <c r="C13" s="24"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="8" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C14" s="8"/>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="8" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8"/>
-      <c r="B16" s="20" t="s">
+      <c r="B16" s="26" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>183</v>
-      </c>
-      <c r="C16" s="8" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="8"/>
-      <c r="B17" s="20"/>
+      <c r="B17" s="26"/>
       <c r="C17" s="8" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="8"/>
-      <c r="B18" s="20"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A19" s="28" t="s">
         <v>186</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A19" s="24" t="s">
-        <v>187</v>
-      </c>
-      <c r="B19" s="24"/>
-      <c r="C19" s="24"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B22" s="8" t="s">
+        <v>191</v>
+      </c>
+      <c r="C22" s="8"/>
+    </row>
+    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A23" s="28" t="s">
         <v>192</v>
       </c>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A23" s="24" t="s">
-        <v>193</v>
-      </c>
-      <c r="B23" s="24"/>
-      <c r="C23" s="24"/>
+      <c r="B23" s="28"/>
+      <c r="C23" s="28"/>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="20" t="s">
+      <c r="A25" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>196</v>
+      </c>
+      <c r="C25" s="8"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="26"/>
+      <c r="B26" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C26" s="8"/>
+    </row>
+    <row r="27" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A27" s="28" t="s">
         <v>197</v>
       </c>
-      <c r="C25" s="8"/>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="20"/>
-      <c r="B26" s="8" t="s">
-        <v>196</v>
-      </c>
-      <c r="C26" s="8"/>
-    </row>
-    <row r="27" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A27" s="24" t="s">
-        <v>198</v>
-      </c>
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
+      <c r="B27" s="28"/>
+      <c r="C27" s="28"/>
     </row>
     <row r="28" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
     </row>
     <row r="31" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A31" s="24" t="s">
-        <v>202</v>
-      </c>
-      <c r="B31" s="24"/>
-      <c r="C31" s="24"/>
+      <c r="A31" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
     </row>
     <row r="32" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
     </row>
     <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
     </row>
     <row r="35" spans="1:4" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="20" t="s">
+      <c r="A35" s="26" t="s">
+        <v>205</v>
+      </c>
+      <c r="B35" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="B35" s="8" t="s">
+      <c r="C35" s="8"/>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="26"/>
+      <c r="B36" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="C35" s="8"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="20"/>
-      <c r="B36" s="8" t="s">
-        <v>208</v>
-      </c>
       <c r="C36" s="8"/>
     </row>
     <row r="37" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A37" s="24" t="s">
-        <v>211</v>
-      </c>
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
+      <c r="A37" s="28" t="s">
+        <v>210</v>
+      </c>
+      <c r="B37" s="28"/>
+      <c r="C37" s="28"/>
     </row>
     <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
+        <v>208</v>
+      </c>
+      <c r="B38" s="8" t="s">
         <v>209</v>
-      </c>
-      <c r="B38" s="8" t="s">
-        <v>210</v>
       </c>
       <c r="C38" s="8"/>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B39" s="8"/>
       <c r="C39" s="8"/>
     </row>
     <row r="40" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
+        <v>212</v>
+      </c>
+      <c r="B40" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="B40" s="8" t="s">
+      <c r="C40" s="8" t="s">
         <v>214</v>
-      </c>
-      <c r="C40" s="8" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B41" s="8"/>
       <c r="C41" s="8"/>
     </row>
     <row r="42" spans="1:4" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20" t="s">
+      <c r="A42" s="26" t="s">
+        <v>216</v>
+      </c>
+      <c r="B42" s="8" t="s">
         <v>217</v>
       </c>
-      <c r="B42" s="8" t="s">
+      <c r="C42" s="29" t="s">
+        <v>220</v>
+      </c>
+      <c r="D42" s="30" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="26"/>
+      <c r="B43" s="8" t="s">
         <v>218</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C43" s="29"/>
+      <c r="D43" s="30"/>
+    </row>
+    <row r="44" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A44" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="D42" s="25" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="20"/>
-      <c r="B43" s="8" t="s">
-        <v>219</v>
-      </c>
-      <c r="C43" s="26"/>
-      <c r="D43" s="25"/>
-    </row>
-    <row r="44" spans="1:4" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A44" s="24" t="s">
-        <v>222</v>
-      </c>
-      <c r="B44" s="24"/>
-      <c r="C44" s="24"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B45" s="8"/>
       <c r="C45" s="8"/>
     </row>
     <row r="46" spans="1:4" ht="135" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="B46" s="8" t="s">
         <v>224</v>
       </c>
-      <c r="B46" s="8" t="s">
+      <c r="C46" s="8" t="s">
         <v>225</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>227</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>228</v>
       </c>
       <c r="C47" s="8"/>
     </row>
     <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B48" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="B48" s="8" t="s">
+      <c r="C48" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="C48" s="8" t="s">
+    </row>
+    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A49" s="28" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="49" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A49" s="24" t="s">
-        <v>232</v>
-      </c>
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
+      <c r="B49" s="28"/>
+      <c r="C49" s="28"/>
     </row>
     <row r="50" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B50" s="8"/>
       <c r="C50" s="8"/>
     </row>
     <row r="51" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B51" s="8"/>
       <c r="C51" s="8"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B52" s="8"/>
       <c r="C52" s="8"/>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B53" s="8"/>
       <c r="C53" s="8"/>
     </row>
     <row r="54" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B54" s="8"/>
       <c r="C54" s="8"/>
     </row>
     <row r="55" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
-        <v>238</v>
-      </c>
-      <c r="B55" s="19"/>
-      <c r="C55" s="19"/>
+      <c r="A55" s="23" t="s">
+        <v>237</v>
+      </c>
+      <c r="B55" s="23"/>
+      <c r="C55" s="23"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B56" s="8" t="s">
         <v>239</v>
-      </c>
-      <c r="B56" s="8" t="s">
-        <v>240</v>
       </c>
       <c r="C56" s="8"/>
     </row>
     <row r="57" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="8" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C57" s="8"/>
     </row>
     <row r="58" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="8" t="s">
+        <v>241</v>
+      </c>
+      <c r="C58" s="8" t="s">
         <v>242</v>
-      </c>
-      <c r="C58" s="8" t="s">
-        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="8"/>
       <c r="B59" s="8"/>
       <c r="C59" s="8" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="60" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="B60" s="8" t="s">
         <v>245</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>246</v>
       </c>
       <c r="C60" s="8"/>
     </row>
     <row r="61" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B61" s="8"/>
       <c r="C61" s="8"/>
     </row>
     <row r="62" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
+        <v>247</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>251</v>
+      </c>
+      <c r="C62" s="8" t="s">
         <v>248</v>
-      </c>
-      <c r="B62" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="C62" s="8" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
+        <v>249</v>
+      </c>
+      <c r="B63" s="8" t="s">
         <v>250</v>
       </c>
-      <c r="B63" s="8" t="s">
-        <v>251</v>
-      </c>
       <c r="C63" s="8" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A64" s="23" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="64" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A64" s="19" t="s">
+      <c r="B64" s="23"/>
+      <c r="C64" s="23"/>
+    </row>
+    <row r="65" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A65" s="28" t="s">
         <v>254</v>
       </c>
-      <c r="B64" s="19"/>
-      <c r="C64" s="19"/>
-    </row>
-    <row r="65" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A65" s="24" t="s">
-        <v>255</v>
-      </c>
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
     </row>
     <row r="66" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A66" s="8" t="s">
+        <v>255</v>
+      </c>
+      <c r="B66" s="8" t="s">
         <v>256</v>
-      </c>
-      <c r="B66" s="8" t="s">
-        <v>257</v>
       </c>
       <c r="C66" s="8"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="8" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C67" s="8"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="8" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C68" s="8"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="C69" s="8"/>
+    </row>
+    <row r="70" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A70" s="28" t="s">
+        <v>261</v>
+      </c>
+      <c r="B70" s="28"/>
+      <c r="C70" s="28"/>
+    </row>
+    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="26" t="s">
         <v>260</v>
       </c>
-      <c r="C69" s="8"/>
-    </row>
-    <row r="70" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A70" s="24" t="s">
+      <c r="B71" s="8" t="s">
         <v>262</v>
       </c>
-      <c r="B70" s="24"/>
-      <c r="C70" s="24"/>
-    </row>
-    <row r="71" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A71" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="B71" s="8" t="s">
+      <c r="C71" s="8"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="26"/>
+      <c r="B72" s="8" t="s">
         <v>263</v>
-      </c>
-      <c r="C71" s="8"/>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="8" t="s">
-        <v>264</v>
       </c>
       <c r="C72" s="8"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="8" t="s">
+        <v>264</v>
+      </c>
+      <c r="B73" s="8" t="s">
         <v>265</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>266</v>
       </c>
       <c r="C73" s="8"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="8"/>
       <c r="B74" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="C74" s="8"/>
+    </row>
+    <row r="75" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A75" s="28" t="s">
         <v>267</v>
       </c>
-      <c r="C74" s="8"/>
-    </row>
-    <row r="75" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
-        <v>268</v>
-      </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="24"/>
+      <c r="B75" s="28"/>
+      <c r="C75" s="28"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="B76" s="8" t="s">
         <v>269</v>
-      </c>
-      <c r="B76" s="8" t="s">
-        <v>270</v>
       </c>
       <c r="C76" s="8"/>
     </row>
     <row r="77" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B77" s="8" t="s">
         <v>272</v>
-      </c>
-      <c r="B77" s="8" t="s">
-        <v>273</v>
       </c>
       <c r="C77" s="8"/>
     </row>
     <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
+        <v>273</v>
+      </c>
+      <c r="B78" s="8" t="s">
         <v>274</v>
       </c>
-      <c r="B78" s="8" t="s">
-        <v>275</v>
-      </c>
       <c r="C78" s="8"/>
     </row>
     <row r="79" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A79" s="24" t="s">
-        <v>282</v>
-      </c>
-      <c r="B79" s="24"/>
-      <c r="C79" s="24"/>
+      <c r="A79" s="28" t="s">
+        <v>281</v>
+      </c>
+      <c r="B79" s="28"/>
+      <c r="C79" s="28"/>
     </row>
     <row r="80" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="B80" s="8" t="s">
         <v>276</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="C80" s="8" t="s">
         <v>277</v>
-      </c>
-      <c r="C80" s="8" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="81" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A81" s="8" t="s">
+        <v>278</v>
+      </c>
+      <c r="B81" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="B81" s="8" t="s">
+      <c r="C81" s="8" t="s">
         <v>280</v>
-      </c>
-      <c r="C81" s="8" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="82" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A82" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B82" s="8" t="s">
         <v>283</v>
-      </c>
-      <c r="B82" s="8" t="s">
-        <v>284</v>
       </c>
       <c r="C82" s="8"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B83" s="8" t="s">
         <v>285</v>
-      </c>
-      <c r="B83" s="8" t="s">
-        <v>286</v>
       </c>
       <c r="C83" s="8"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="8" t="s">
+        <v>286</v>
+      </c>
+      <c r="C84" s="8"/>
+    </row>
+    <row r="85" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A85" s="28" t="s">
         <v>287</v>
       </c>
-      <c r="C84" s="8"/>
-    </row>
-    <row r="85" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A85" s="24" t="s">
-        <v>288</v>
-      </c>
-      <c r="B85" s="24"/>
-      <c r="C85" s="24"/>
+      <c r="B85" s="28"/>
+      <c r="C85" s="28"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="8" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C86" s="8"/>
     </row>
     <row r="87" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A87" s="8" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B87" s="8" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C87" s="8"/>
     </row>
     <row r="88" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A88" s="8" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B88" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="C88" s="8"/>
+    </row>
+    <row r="89" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A89" s="28" t="s">
         <v>294</v>
       </c>
-      <c r="C88" s="8"/>
-    </row>
-    <row r="89" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A89" s="24" t="s">
-        <v>295</v>
-      </c>
-      <c r="B89" s="24"/>
-      <c r="C89" s="24"/>
+      <c r="B89" s="28"/>
+      <c r="C89" s="28"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="8" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B90" s="8"/>
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="20" t="s">
+      <c r="A91" s="26" t="s">
+        <v>296</v>
+      </c>
+      <c r="B91" s="8" t="s">
         <v>297</v>
       </c>
-      <c r="B91" s="8" t="s">
+      <c r="C91" s="8"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="26"/>
+      <c r="B92" s="8" t="s">
         <v>298</v>
-      </c>
-      <c r="C91" s="8"/>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="20"/>
-      <c r="B92" s="8" t="s">
-        <v>299</v>
       </c>
       <c r="C92" s="8"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="B93" s="8"/>
       <c r="C93" s="8"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="16" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B94" s="8"/>
       <c r="C94" s="8"/>
     </row>
     <row r="95" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A95" s="19" t="s">
-        <v>302</v>
-      </c>
-      <c r="B95" s="19"/>
-      <c r="C95" s="19"/>
+      <c r="A95" s="23" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" s="23"/>
+      <c r="C95" s="23"/>
     </row>
     <row r="96" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A96" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="B96" s="8" t="s">
         <v>303</v>
-      </c>
-      <c r="B96" s="8" t="s">
-        <v>304</v>
       </c>
       <c r="C96" s="8"/>
     </row>
     <row r="97" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A97" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="B97" s="8" t="s">
         <v>305</v>
       </c>
-      <c r="B97" s="8" t="s">
+      <c r="C97" s="8" t="s">
         <v>306</v>
       </c>
-      <c r="C97" s="8" t="s">
+    </row>
+    <row r="98" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
+      <c r="A98" s="28" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="98" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A98" s="24" t="s">
+      <c r="B98" s="28"/>
+      <c r="C98" s="28"/>
+    </row>
+    <row r="99" spans="1:3" ht="195" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A99" s="30" t="s">
+        <v>309</v>
+      </c>
+      <c r="B99" s="30"/>
+      <c r="C99" s="8" t="s">
         <v>308</v>
       </c>
-      <c r="B98" s="24"/>
-      <c r="C98" s="24"/>
-    </row>
-    <row r="99" spans="1:3" ht="195" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="25" t="s">
-        <v>310</v>
-      </c>
-      <c r="B99" s="25"/>
-      <c r="C99" s="8" t="s">
-        <v>309</v>
-      </c>
     </row>
     <row r="100" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="24" t="s">
-        <v>314</v>
-      </c>
-      <c r="B100" s="24"/>
-      <c r="C100" s="24"/>
+      <c r="A100" s="28" t="s">
+        <v>313</v>
+      </c>
+      <c r="B100" s="28"/>
+      <c r="C100" s="28"/>
     </row>
     <row r="101" spans="1:3" ht="165" x14ac:dyDescent="0.25">
       <c r="A101" s="8" t="s">
+        <v>310</v>
+      </c>
+      <c r="B101" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="C101" s="8" t="s">
         <v>311</v>
       </c>
-      <c r="B101" s="8" t="s">
-        <v>313</v>
-      </c>
-      <c r="C101" s="8" t="s">
-        <v>312</v>
-      </c>
     </row>
     <row r="102" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A102" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="B102" s="24"/>
-      <c r="C102" s="24"/>
+      <c r="A102" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="B102" s="28"/>
+      <c r="C102" s="28"/>
     </row>
     <row r="103" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A103" s="8" t="s">
+        <v>315</v>
+      </c>
+      <c r="B103" s="8" t="s">
         <v>316</v>
       </c>
-      <c r="B103" s="8" t="s">
+      <c r="C103" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="C103" s="8" t="s">
-        <v>318</v>
-      </c>
     </row>
     <row r="104" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A104" s="24" t="s">
-        <v>315</v>
-      </c>
-      <c r="B104" s="24"/>
-      <c r="C104" s="24"/>
+      <c r="A104" s="28" t="s">
+        <v>314</v>
+      </c>
+      <c r="B104" s="28"/>
+      <c r="C104" s="28"/>
     </row>
     <row r="105" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="B105" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="B105" s="8" t="s">
-        <v>320</v>
-      </c>
       <c r="C105" s="8"/>
     </row>
     <row r="106" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A106" s="19"/>
-      <c r="B106" s="19"/>
-      <c r="C106" s="19"/>
+      <c r="A106" s="23"/>
+      <c r="B106" s="23"/>
+      <c r="C106" s="23"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="8"/>
@@ -4685,6 +4763,29 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="A106:C106"/>
+    <mergeCell ref="A98:C98"/>
+    <mergeCell ref="A99:B99"/>
+    <mergeCell ref="A100:C100"/>
+    <mergeCell ref="A102:C102"/>
+    <mergeCell ref="A104:C104"/>
+    <mergeCell ref="A95:C95"/>
+    <mergeCell ref="A49:C49"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="A64:C64"/>
+    <mergeCell ref="A65:C65"/>
+    <mergeCell ref="A70:C70"/>
+    <mergeCell ref="A71:A72"/>
+    <mergeCell ref="A75:C75"/>
+    <mergeCell ref="A79:C79"/>
+    <mergeCell ref="A85:C85"/>
+    <mergeCell ref="A89:C89"/>
+    <mergeCell ref="A91:A92"/>
+    <mergeCell ref="A37:C37"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="A44:C44"/>
     <mergeCell ref="A35:A36"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="A2:C2"/>
@@ -4697,29 +4798,6 @@
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="B16:B18"/>
     <mergeCell ref="A31:C31"/>
-    <mergeCell ref="A37:C37"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="D42:D43"/>
-    <mergeCell ref="A44:C44"/>
-    <mergeCell ref="A95:C95"/>
-    <mergeCell ref="A49:C49"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="A64:C64"/>
-    <mergeCell ref="A65:C65"/>
-    <mergeCell ref="A70:C70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A75:C75"/>
-    <mergeCell ref="A79:C79"/>
-    <mergeCell ref="A85:C85"/>
-    <mergeCell ref="A89:C89"/>
-    <mergeCell ref="A91:A92"/>
-    <mergeCell ref="A106:C106"/>
-    <mergeCell ref="A98:C98"/>
-    <mergeCell ref="A99:B99"/>
-    <mergeCell ref="A100:C100"/>
-    <mergeCell ref="A102:C102"/>
-    <mergeCell ref="A104:C104"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="A93" r:id="rId1" display="https://blog.angular-university.io/functional-reactive-programming-for-angular-2-developers-rxjs-and-observables/"/>

</xml_diff>